<commit_message>
hotfix verificar menor qtd do produto
</commit_message>
<xml_diff>
--- a/bot/Assets/IO/Input/Execucao.xlsx
+++ b/bot/Assets/IO/Input/Execucao.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bot-clicker-orcamento\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronaldo.buscarini\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="15372" windowHeight="7968"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8952"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -19,361 +19,47 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Produto</t>
-  </si>
-  <si>
-    <t>QUERAZEN</t>
-  </si>
-  <si>
-    <t>CLARITROMICINA</t>
-  </si>
-  <si>
-    <t>MODUKINE</t>
-  </si>
-  <si>
-    <t>PEAK ATP</t>
-  </si>
-  <si>
-    <t>AC CITRICO</t>
-  </si>
-  <si>
-    <t>HIBISCUS EXT SECO</t>
-  </si>
-  <si>
-    <t>TEACRINE</t>
   </si>
   <si>
     <t>Quantidade</t>
   </si>
   <si>
-    <t>BETACAROTENO</t>
+    <t>Bromoprida</t>
   </si>
   <si>
-    <t>AC ACETICO</t>
+    <t>Deflazacort</t>
   </si>
   <si>
-    <t>AC FITICO</t>
+    <t>Dustasterida</t>
   </si>
   <si>
-    <t>AC HIALURONICO (P/ CAPSULAS)</t>
+    <t>Terbinafina</t>
   </si>
   <si>
-    <t>ACETATO CIPROTERONA</t>
+    <t>SAME</t>
   </si>
   <si>
-    <t>AGNUS CASTUS</t>
+    <t>Passiflora</t>
   </si>
   <si>
-    <t>ARGININA AKG</t>
+    <t>Açafrão</t>
   </si>
   <si>
-    <t>AZATIOPRINA</t>
+    <t>Vit D</t>
   </si>
   <si>
-    <t>BASE EFERVECENTE</t>
+    <t>Carbotil UG</t>
   </si>
   <si>
-    <t>BASE P/ SUPOSITÓRIO</t>
-  </si>
-  <si>
-    <t>BETA VULGARIS</t>
-  </si>
-  <si>
-    <t>BETAINA HCL</t>
-  </si>
-  <si>
-    <t>CALCIO QUELADO</t>
-  </si>
-  <si>
-    <t>CANFORA</t>
-  </si>
-  <si>
-    <t>CAP ENTERICA - 00</t>
-  </si>
-  <si>
-    <t>CAP ENTERICA - 1</t>
-  </si>
-  <si>
-    <t>CAP ENTERICA - 2</t>
-  </si>
-  <si>
-    <t>CAP ENTERICA - 3</t>
-  </si>
-  <si>
-    <t>CAP GELAT - 2 - (AZUL/BRANCO)</t>
-  </si>
-  <si>
-    <t>CAP GELAT - 2 - (ESCARL/BRANCA</t>
-  </si>
-  <si>
-    <t>CAP GELAT - 2 - (VERDE/BRANCA)</t>
-  </si>
-  <si>
-    <t>CAP GELAT - 3 - (AZUL/BRANCA)</t>
-  </si>
-  <si>
-    <t>CAP GELAT - 3 - (ESCAR/BRANC)</t>
-  </si>
-  <si>
-    <t>CAP GELAT - 3 - (VERDE/BRANCO)</t>
-  </si>
-  <si>
-    <t>CAP VEGETAL - 2 - (BRANCA)</t>
-  </si>
-  <si>
-    <t>CARBONATO DE CALCIO</t>
-  </si>
-  <si>
-    <t>CLORELLA</t>
-  </si>
-  <si>
-    <t>CLOREXIDINA</t>
-  </si>
-  <si>
-    <t>CLOROQUINA</t>
-  </si>
-  <si>
-    <t>D PANTOTENATO CALCIO</t>
-  </si>
-  <si>
-    <t>DEFLAZACORT</t>
-  </si>
-  <si>
-    <t>DL METIONINA</t>
-  </si>
-  <si>
-    <t>DMAE (C/BITARTARATO)</t>
-  </si>
-  <si>
-    <t>DMSO</t>
-  </si>
-  <si>
-    <t>DOXICICLINA</t>
-  </si>
-  <si>
-    <t>EFADERMA</t>
-  </si>
-  <si>
-    <t>ENTEROCOCCUS FAECIUM</t>
-  </si>
-  <si>
-    <t>ESTRIOL MP</t>
-  </si>
-  <si>
-    <t>ESTROGENOS CONJUGADOS</t>
-  </si>
-  <si>
-    <t>EXT GLICOL CAST INDIA</t>
-  </si>
-  <si>
-    <t>EXT GLICOL GINKGO BILOBA</t>
-  </si>
-  <si>
-    <t>FENILALANINA</t>
-  </si>
-  <si>
-    <t>FOSFATIDILSERINA</t>
-  </si>
-  <si>
-    <t>GARCINIA</t>
-  </si>
-  <si>
-    <t>GLUTATION REDUZIDO</t>
-  </si>
-  <si>
-    <t>GLYCOXIL</t>
-  </si>
-  <si>
-    <t>GUARANA EXT SECO</t>
-  </si>
-  <si>
-    <t>HEXANICOTINATO DE INOSITOL</t>
-  </si>
-  <si>
-    <t>HIDROXICLOROQUINA</t>
-  </si>
-  <si>
-    <t>HIDROXIPROLISILANE C</t>
-  </si>
-  <si>
-    <t>HMB CA</t>
-  </si>
-  <si>
-    <t>HRT HEAVY GEL TRANSDERMICO</t>
-  </si>
-  <si>
-    <t>INDOL 3 CARBINOL</t>
-  </si>
-  <si>
-    <t>ISOLEUCINA</t>
-  </si>
-  <si>
-    <t>ITRACONAZOL</t>
-  </si>
-  <si>
-    <t>LACTOBACILLUS SPOROGENES</t>
-  </si>
-  <si>
-    <t>LANOLINA</t>
-  </si>
-  <si>
-    <t>LEUCINA</t>
-  </si>
-  <si>
-    <t>LIPASE</t>
-  </si>
-  <si>
-    <t>LISINA</t>
-  </si>
-  <si>
-    <t>LOSARTAN</t>
-  </si>
-  <si>
-    <t>LUTEINA</t>
-  </si>
-  <si>
-    <t>MACA</t>
-  </si>
-  <si>
-    <t>MAGNESIO TREONATO</t>
-  </si>
-  <si>
-    <t>MELISSA</t>
-  </si>
-  <si>
-    <t>MENTOL</t>
-  </si>
-  <si>
-    <t>METIMAZOL</t>
-  </si>
-  <si>
-    <t>METOTREXATO MP</t>
-  </si>
-  <si>
-    <t>MIO INOSITOL</t>
-  </si>
-  <si>
-    <t>MOMETASONA FUROATO MP</t>
-  </si>
-  <si>
-    <t>MOVE</t>
-  </si>
-  <si>
-    <t>NICOTINAMIDA</t>
-  </si>
-  <si>
-    <t>NORVALINA</t>
-  </si>
-  <si>
-    <t>OL AMENDOAS DOCE</t>
-  </si>
-  <si>
-    <t>OLI OLA (PEELING CAPSULA)</t>
-  </si>
-  <si>
-    <t>PAPAINA</t>
-  </si>
-  <si>
-    <t>PASSIFLORA</t>
-  </si>
-  <si>
-    <t>PENTRAVAM</t>
-  </si>
-  <si>
-    <t>PIGMERISE</t>
-  </si>
-  <si>
-    <t>PIMOBENDAM MP</t>
-  </si>
-  <si>
-    <t>PIRIDOXAL 5-FOSFATO</t>
-  </si>
-  <si>
-    <t>POLIQUATERNARIO 7</t>
-  </si>
-  <si>
-    <t>PROGESTERONA</t>
-  </si>
-  <si>
-    <t>PROTETOR FPS 45 EXTRA-SECO FIN</t>
-  </si>
-  <si>
-    <t>PSYLLIUM</t>
-  </si>
-  <si>
-    <t>SELENIO QUELADO</t>
-  </si>
-  <si>
-    <t>SERENZO</t>
-  </si>
-  <si>
-    <t>SERTRALINA (COMO HCL)</t>
-  </si>
-  <si>
-    <t>SILIMARINA</t>
-  </si>
-  <si>
-    <t>SLIM FIBER</t>
-  </si>
-  <si>
-    <t>SOLUVET PICANHA</t>
-  </si>
-  <si>
-    <t>SULBUTIAMINA</t>
-  </si>
-  <si>
-    <t>TADALAFIL</t>
-  </si>
-  <si>
-    <t>TEACRINA GENERICO</t>
-  </si>
-  <si>
-    <t>TENOXICAM</t>
-  </si>
-  <si>
-    <t>TESTOSTERONA BIOIDENTICA MP</t>
-  </si>
-  <si>
-    <t>TINT ALECRIM</t>
-  </si>
-  <si>
-    <t>TINT COENTRO</t>
-  </si>
-  <si>
-    <t>TINT GUACATONGA</t>
-  </si>
-  <si>
-    <t>TIROSINA</t>
-  </si>
-  <si>
-    <t>VEGF (FATOR CRESC ENDO VASCULA</t>
-  </si>
-  <si>
-    <t>VIT E OLEO (TOPICA)</t>
-  </si>
-  <si>
-    <t>VITACOLOR AR</t>
-  </si>
-  <si>
-    <t>YOIMBINA HCL MP</t>
-  </si>
-  <si>
-    <t>PEPSINA</t>
+    <t>Cápsula 00 Incolor</t>
   </si>
 </sst>
 </file>
@@ -384,7 +70,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +167,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -543,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -570,6 +262,7 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,7 +547,7 @@
   <dimension ref="A1:F891"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,686 +562,481 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>9</v>
+      <c r="A2" s="15" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>10</v>
+      <c r="A3" s="15" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>11</v>
-      </c>
       <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>12</v>
+      <c r="A6" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="15"/>
       <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>13</v>
+      <c r="A7" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>14</v>
+      <c r="A8" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>15</v>
+      <c r="A9" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>16</v>
+      <c r="A10" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>17</v>
+      <c r="A11" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="B11" s="15"/>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="A12" s="10"/>
       <c r="B12" s="15"/>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="A13" s="10"/>
       <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="A14" s="10"/>
       <c r="B14" s="15"/>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="A15" s="10"/>
       <c r="B15" s="15"/>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="A16" s="10"/>
       <c r="B16" s="15"/>
+      <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="A17" s="10"/>
       <c r="B17" s="15"/>
     </row>
     <row r="18" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="A18" s="10"/>
       <c r="B18" s="15"/>
     </row>
     <row r="19" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="A19" s="10"/>
       <c r="B19" s="15"/>
     </row>
     <row r="20" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="A20" s="10"/>
       <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="A21" s="10"/>
       <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="A22" s="10"/>
       <c r="B22" s="15"/>
     </row>
     <row r="23" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="A23" s="10"/>
       <c r="B23" s="15"/>
     </row>
     <row r="24" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>29</v>
-      </c>
+      <c r="A24" s="10"/>
       <c r="B24" s="15"/>
     </row>
     <row r="25" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="A25" s="10"/>
       <c r="B25" s="15"/>
     </row>
     <row r="26" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="A26" s="10"/>
       <c r="B26" s="15"/>
     </row>
     <row r="27" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>32</v>
-      </c>
+      <c r="A27" s="10"/>
       <c r="B27" s="15"/>
     </row>
     <row r="28" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="A28" s="10"/>
       <c r="B28" s="15"/>
     </row>
     <row r="29" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>34</v>
-      </c>
+      <c r="A29" s="10"/>
       <c r="B29" s="15"/>
     </row>
     <row r="30" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
-        <v>2</v>
-      </c>
+      <c r="A30" s="10"/>
       <c r="B30" s="15"/>
     </row>
     <row r="31" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="A31" s="10"/>
       <c r="B31" s="15"/>
     </row>
     <row r="32" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="A32" s="10"/>
       <c r="B32" s="15"/>
     </row>
     <row r="33" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="A33" s="10"/>
       <c r="B33" s="15"/>
     </row>
     <row r="34" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="A34" s="10"/>
       <c r="B34" s="15"/>
     </row>
     <row r="35" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="A35" s="10"/>
       <c r="B35" s="15"/>
     </row>
     <row r="36" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="A36" s="10"/>
       <c r="B36" s="15"/>
     </row>
     <row r="37" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="A37" s="10"/>
       <c r="B37" s="15"/>
     </row>
     <row r="38" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="A38" s="10"/>
       <c r="B38" s="15"/>
     </row>
     <row r="39" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="A39" s="10"/>
       <c r="B39" s="15"/>
     </row>
     <row r="40" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="A40" s="10"/>
       <c r="B40" s="15"/>
     </row>
     <row r="41" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="A41" s="10"/>
       <c r="B41" s="15"/>
     </row>
     <row r="42" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="A42" s="10"/>
       <c r="B42" s="15"/>
     </row>
     <row r="43" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
-        <v>47</v>
-      </c>
+      <c r="A43" s="10"/>
       <c r="B43" s="15"/>
     </row>
     <row r="44" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>48</v>
-      </c>
+      <c r="A44" s="10"/>
       <c r="B44" s="15"/>
     </row>
     <row r="45" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="A45" s="10"/>
       <c r="B45" s="15"/>
     </row>
     <row r="46" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="A46" s="10"/>
       <c r="B46" s="15"/>
     </row>
     <row r="47" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="A47" s="10"/>
       <c r="B47" s="15"/>
     </row>
     <row r="48" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="A48" s="10"/>
       <c r="B48" s="15"/>
     </row>
     <row r="49" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="A49" s="10"/>
       <c r="B49" s="15"/>
     </row>
     <row r="50" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="A50" s="10"/>
       <c r="B50" s="15"/>
     </row>
     <row r="51" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
-        <v>55</v>
-      </c>
+      <c r="A51" s="10"/>
       <c r="B51" s="15"/>
     </row>
     <row r="52" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
-        <v>56</v>
-      </c>
+      <c r="A52" s="10"/>
       <c r="B52" s="15"/>
     </row>
     <row r="53" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="A53" s="10"/>
       <c r="B53" s="15"/>
     </row>
     <row r="54" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="A54" s="10"/>
       <c r="B54" s="15"/>
     </row>
     <row r="55" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="A55" s="10"/>
       <c r="B55" s="15"/>
     </row>
     <row r="56" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="s">
-        <v>59</v>
-      </c>
+      <c r="A56" s="10"/>
       <c r="B56" s="15"/>
     </row>
     <row r="57" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>60</v>
-      </c>
+      <c r="A57" s="10"/>
       <c r="B57" s="15"/>
     </row>
     <row r="58" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="A58" s="10"/>
       <c r="B58" s="15"/>
     </row>
     <row r="59" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="A59" s="10"/>
       <c r="B59" s="15"/>
     </row>
     <row r="60" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="A60" s="10"/>
       <c r="B60" s="15"/>
     </row>
     <row r="61" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
-        <v>64</v>
-      </c>
+      <c r="A61" s="10"/>
       <c r="B61" s="15"/>
     </row>
     <row r="62" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="s">
-        <v>65</v>
-      </c>
+      <c r="A62" s="10"/>
       <c r="B62" s="15"/>
     </row>
     <row r="63" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="s">
-        <v>66</v>
-      </c>
+      <c r="A63" s="10"/>
       <c r="B63" s="15"/>
     </row>
     <row r="64" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="s">
-        <v>67</v>
-      </c>
+      <c r="A64" s="10"/>
       <c r="B64" s="15"/>
     </row>
     <row r="65" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="s">
-        <v>68</v>
-      </c>
+      <c r="A65" s="10"/>
       <c r="B65" s="15"/>
     </row>
     <row r="66" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="10" t="s">
-        <v>69</v>
-      </c>
+      <c r="A66" s="10"/>
       <c r="B66" s="15"/>
     </row>
     <row r="67" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="10" t="s">
-        <v>70</v>
-      </c>
+      <c r="A67" s="10"/>
       <c r="B67" s="15"/>
     </row>
     <row r="68" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="10" t="s">
-        <v>71</v>
-      </c>
+      <c r="A68" s="10"/>
       <c r="B68" s="15"/>
     </row>
     <row r="69" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="A69" s="10"/>
       <c r="B69" s="15"/>
     </row>
     <row r="70" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="10" t="s">
-        <v>73</v>
-      </c>
+      <c r="A70" s="10"/>
       <c r="B70" s="15"/>
     </row>
     <row r="71" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="10" t="s">
-        <v>74</v>
-      </c>
+      <c r="A71" s="10"/>
       <c r="B71" s="15"/>
     </row>
     <row r="72" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="10" t="s">
-        <v>75</v>
-      </c>
+      <c r="A72" s="10"/>
       <c r="B72" s="15"/>
     </row>
     <row r="73" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="10" t="s">
-        <v>76</v>
-      </c>
+      <c r="A73" s="10"/>
       <c r="B73" s="15"/>
     </row>
     <row r="74" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="s">
-        <v>77</v>
-      </c>
+      <c r="A74" s="10"/>
       <c r="B74" s="15"/>
     </row>
     <row r="75" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="A75" s="10"/>
       <c r="B75" s="15"/>
     </row>
     <row r="76" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="10" t="s">
-        <v>78</v>
-      </c>
+      <c r="A76" s="10"/>
       <c r="B76" s="15"/>
     </row>
     <row r="77" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="10" t="s">
-        <v>79</v>
-      </c>
+      <c r="A77" s="10"/>
       <c r="B77" s="15"/>
     </row>
     <row r="78" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="10" t="s">
-        <v>80</v>
-      </c>
+      <c r="A78" s="10"/>
       <c r="B78" s="15"/>
     </row>
     <row r="79" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="10" t="s">
-        <v>81</v>
-      </c>
+      <c r="A79" s="10"/>
       <c r="B79" s="15"/>
     </row>
     <row r="80" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="10" t="s">
-        <v>82</v>
-      </c>
+      <c r="A80" s="10"/>
       <c r="B80" s="15"/>
     </row>
     <row r="81" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="10" t="s">
-        <v>83</v>
-      </c>
+      <c r="A81" s="10"/>
       <c r="B81" s="15"/>
     </row>
     <row r="82" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="10" t="s">
-        <v>84</v>
-      </c>
+      <c r="A82" s="10"/>
       <c r="B82" s="15"/>
     </row>
     <row r="83" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="10" t="s">
-        <v>85</v>
-      </c>
+      <c r="A83" s="10"/>
       <c r="B83" s="15"/>
     </row>
     <row r="84" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="A84" s="10"/>
       <c r="B84" s="15"/>
     </row>
     <row r="85" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="10" t="s">
-        <v>86</v>
-      </c>
+      <c r="A85" s="10"/>
       <c r="B85" s="15"/>
     </row>
     <row r="86" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="10" t="s">
-        <v>87</v>
-      </c>
+      <c r="A86" s="10"/>
       <c r="B86" s="15"/>
     </row>
     <row r="87" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="10" t="s">
-        <v>88</v>
-      </c>
+      <c r="A87" s="10"/>
       <c r="B87" s="15"/>
     </row>
     <row r="88" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="10" t="s">
-        <v>89</v>
-      </c>
+      <c r="A88" s="10"/>
       <c r="B88" s="15"/>
     </row>
     <row r="89" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="A89" s="10"/>
       <c r="B89" s="15"/>
     </row>
     <row r="90" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A90" s="10"/>
       <c r="B90" s="15"/>
     </row>
     <row r="91" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="s">
-        <v>92</v>
-      </c>
+      <c r="A91" s="10"/>
       <c r="B91" s="15"/>
     </row>
     <row r="92" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="10" t="s">
-        <v>93</v>
-      </c>
+      <c r="A92" s="10"/>
       <c r="B92" s="15"/>
     </row>
     <row r="93" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="10" t="s">
-        <v>1</v>
-      </c>
+      <c r="A93" s="10"/>
       <c r="B93" s="15"/>
     </row>
     <row r="94" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="10" t="s">
-        <v>94</v>
-      </c>
+      <c r="A94" s="10"/>
       <c r="B94" s="15"/>
     </row>
     <row r="95" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="10" t="s">
-        <v>95</v>
-      </c>
+      <c r="A95" s="10"/>
       <c r="B95" s="15"/>
     </row>
     <row r="96" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="A96" s="10"/>
       <c r="B96" s="15"/>
     </row>
     <row r="97" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="10" t="s">
-        <v>97</v>
-      </c>
+      <c r="A97" s="10"/>
       <c r="B97" s="15"/>
     </row>
     <row r="98" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="s">
-        <v>98</v>
-      </c>
+      <c r="A98" s="10"/>
       <c r="B98" s="15"/>
     </row>
     <row r="99" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="10" t="s">
-        <v>99</v>
-      </c>
+      <c r="A99" s="10"/>
       <c r="B99" s="15"/>
     </row>
     <row r="100" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="10" t="s">
-        <v>100</v>
-      </c>
+      <c r="A100" s="10"/>
       <c r="B100" s="15"/>
     </row>
     <row r="101" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="A101" s="10"/>
       <c r="B101" s="15"/>
     </row>
     <row r="102" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="10" t="s">
-        <v>102</v>
-      </c>
+      <c r="A102" s="10"/>
       <c r="B102" s="15"/>
     </row>
     <row r="103" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="A103" s="10"/>
       <c r="B103" s="15"/>
     </row>
     <row r="104" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A104" s="10"/>
       <c r="B104" s="15"/>
     </row>
     <row r="105" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="10" t="s">
-        <v>104</v>
-      </c>
+      <c r="A105" s="10"/>
       <c r="B105" s="15"/>
     </row>
     <row r="106" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="10" t="s">
-        <v>105</v>
-      </c>
+      <c r="A106" s="10"/>
       <c r="B106" s="15"/>
     </row>
     <row r="107" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="10" t="s">
-        <v>106</v>
-      </c>
+      <c r="A107" s="10"/>
       <c r="B107" s="15"/>
     </row>
     <row r="108" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="A108" s="10"/>
       <c r="B108" s="15"/>
     </row>
     <row r="109" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="10" t="s">
-        <v>108</v>
-      </c>
+      <c r="A109" s="10"/>
       <c r="B109" s="15"/>
     </row>
     <row r="110" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="10" t="s">
-        <v>109</v>
-      </c>
+      <c r="A110" s="10"/>
       <c r="B110" s="15"/>
     </row>
     <row r="111" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="10" t="s">
-        <v>110</v>
-      </c>
+      <c r="A111" s="10"/>
       <c r="B111" s="15"/>
     </row>
     <row r="112" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="10" t="s">
-        <v>111</v>
-      </c>
+      <c r="A112" s="10"/>
       <c r="B112" s="15"/>
     </row>
     <row r="113" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="10" t="s">
-        <v>112</v>
-      </c>
+      <c r="A113" s="10"/>
       <c r="B113" s="15"/>
     </row>
     <row r="114" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="10" t="s">
-        <v>113</v>
-      </c>
+      <c r="A114" s="10"/>
       <c r="B114" s="15"/>
     </row>
     <row r="115" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
correções de execução do bot
</commit_message>
<xml_diff>
--- a/bot/Assets/IO/Input/Execucao.xlsx
+++ b/bot/Assets/IO/Input/Execucao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bot-clicker-orcamento\bot\Assets\IO\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Produto</t>
   </si>
@@ -32,199 +32,16 @@
     <t>Quantidade</t>
   </si>
   <si>
-    <t>CHÁ VERDE</t>
+    <t>LACTOBACILUS CASEI</t>
   </si>
   <si>
-    <t>HAMAMELIS</t>
+    <t>LACTOBACILUS PLANTARUM</t>
   </si>
   <si>
-    <t>COMPLEX</t>
+    <t>LACTOBACILUS SALIVARIUM</t>
   </si>
   <si>
-    <t>Acetil metionina / I metionina</t>
-  </si>
-  <si>
-    <t>BASE CREME VAGINAL VENCE DIA 01/10/2022</t>
-  </si>
-  <si>
-    <t>BIOENXOFRE</t>
-  </si>
-  <si>
-    <t>Bifiddobacterium Infantis</t>
-  </si>
-  <si>
-    <t>Carob Active (extrato seco de Alfarroba)</t>
-  </si>
-  <si>
-    <t>Ciprofibrato</t>
-  </si>
-  <si>
-    <t>DENSISKIN D+</t>
-  </si>
-  <si>
-    <t>Doxepina HCl</t>
-  </si>
-  <si>
-    <t>DL Carnitina HCl</t>
-  </si>
-  <si>
-    <t>ESMALTE HIPOALERGENICO</t>
-  </si>
-  <si>
-    <t>ESTAGEL (SEPIGEL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTRATO GLICOLICO DE </t>
-  </si>
-  <si>
-    <t>Fabenol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLAVORIZANTE DE  </t>
-  </si>
-  <si>
-    <t>BAUNILHA PO</t>
-  </si>
-  <si>
-    <t>FLAVORIZANTE DE CHOCOLATE PO</t>
-  </si>
-  <si>
-    <t>FLAVORIZANTE DE FRAMBOESA PO</t>
-  </si>
-  <si>
-    <t>FLAVORIZANTE DE LARANJA PO</t>
-  </si>
-  <si>
-    <t>FLAVORIZANTE DE LIMAO PO</t>
-  </si>
-  <si>
-    <t>FLAVORIZANTE DE MORANGO</t>
-  </si>
-  <si>
-    <t>FLAVORIZANTE DE UVA PO ( COMPRAR NO LUGAR DO REFRESCO DE UVA)</t>
-  </si>
-  <si>
-    <t>FRESCOLAT</t>
-  </si>
-  <si>
-    <t>Glisodin</t>
-  </si>
-  <si>
-    <t>GLUCAMATE DOE 120</t>
-  </si>
-  <si>
-    <t>GLUCAMATE LT</t>
-  </si>
-  <si>
-    <t>LECIGEL</t>
-  </si>
-  <si>
-    <t>LUMINECENSE</t>
-  </si>
-  <si>
-    <t>Levemax (Rubus Fruticosos Extrato)</t>
-  </si>
-  <si>
-    <t>Luterana</t>
-  </si>
-  <si>
-    <t>Magnesio Inositol</t>
-  </si>
-  <si>
-    <t>Metabolise 4</t>
-  </si>
-  <si>
-    <t>METOXISALENO</t>
-  </si>
-  <si>
-    <t>Minociclina HCl</t>
-  </si>
-  <si>
-    <t>Mobilee</t>
-  </si>
-  <si>
-    <t>Naltrexona</t>
-  </si>
-  <si>
-    <t>Niacina (Ácido Nicotinico)</t>
-  </si>
-  <si>
-    <t>Nicotinato de Inositol</t>
-  </si>
-  <si>
-    <t>NICOTINAMIDA PC</t>
-  </si>
-  <si>
-    <t>NICOTINATO DE METILA</t>
-  </si>
-  <si>
-    <t>OCTOPIROX OLAMINA (PIROCTONA OLAMINA)</t>
-  </si>
-  <si>
-    <t>OLEO DE COPAÍBA</t>
-  </si>
-  <si>
-    <t>Óleo de Oliva</t>
-  </si>
-  <si>
-    <t>Ômega 3 pó</t>
-  </si>
-  <si>
-    <t>Opuntia Ficus Indica</t>
-  </si>
-  <si>
-    <t>Ornitina Alfacetaglutarato</t>
-  </si>
-  <si>
-    <t>Pancreatina pó</t>
-  </si>
-  <si>
-    <t>Pholoridzin</t>
-  </si>
-  <si>
-    <t>PINETONINA</t>
-  </si>
-  <si>
-    <t>POLIETILENOGLICOL 300</t>
-  </si>
-  <si>
-    <t>PROPILENOGLICOL</t>
-  </si>
-  <si>
-    <t>REVINAGE</t>
-  </si>
-  <si>
-    <t>Serenzo</t>
-  </si>
-  <si>
-    <t>Streptococus Faecium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKIN WHITENING </t>
-  </si>
-  <si>
-    <t>SORBATO DE POTASSIO</t>
-  </si>
-  <si>
-    <t>STEVIA PO</t>
-  </si>
-  <si>
-    <t>SYRSPEND ALKA DRG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TINTURA DE PROPOLIS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TINTURA GYMENA </t>
-  </si>
-  <si>
-    <t>SYLVESTRE</t>
-  </si>
-  <si>
-    <t>UCON FLUID AP</t>
-  </si>
-  <si>
-    <t>VEEGUM ULTRA</t>
+    <t>PIRIDOXINA</t>
   </si>
 </sst>
 </file>
@@ -235,7 +52,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,21 +140,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -400,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -426,8 +228,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -711,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I891"/>
+  <dimension ref="A1:I773"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +522,7 @@
     <col min="1" max="1" width="41.33203125" style="8" customWidth="1"/>
     <col min="2" max="2" width="32.44140625" style="9" customWidth="1"/>
     <col min="3" max="8" width="9.109375" style="3"/>
-    <col min="9" max="9" width="48.77734375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.77734375" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
@@ -735,2529 +535,2287 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="15"/>
-      <c r="I2" s="20"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>6</v>
+      <c r="A3" s="10" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="15"/>
-      <c r="I3" s="20"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>7</v>
+      <c r="A4" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="I4" s="20"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>8</v>
+      <c r="A5" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="I5" s="20"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>9</v>
+      <c r="A6" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="B6" s="15"/>
-      <c r="F6" s="17"/>
-      <c r="I6" s="20"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="A7" s="10"/>
       <c r="B7" s="15"/>
-      <c r="I7" s="20"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="A8" s="10"/>
       <c r="B8" s="15"/>
-      <c r="I8" s="20"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="A9" s="10"/>
       <c r="B9" s="15"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
-        <v>13</v>
-      </c>
+      <c r="A10" s="10"/>
       <c r="B10" s="15"/>
-      <c r="I10" s="20"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
-        <v>14</v>
-      </c>
+      <c r="A11" s="10"/>
       <c r="B11" s="15"/>
-      <c r="I11" s="20"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="A12" s="10"/>
       <c r="B12" s="15"/>
-      <c r="I12" s="20"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="A13" s="10"/>
       <c r="B13" s="15"/>
-      <c r="I13" s="20"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>2</v>
-      </c>
+      <c r="A14" s="10"/>
       <c r="B14" s="15"/>
-      <c r="I14" s="20"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="A15" s="10"/>
       <c r="B15" s="15"/>
-      <c r="I15" s="20"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>3</v>
-      </c>
+      <c r="A16" s="10"/>
       <c r="B16" s="15"/>
-      <c r="D16" s="18"/>
-      <c r="I16" s="20"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
-        <v>17</v>
-      </c>
+      <c r="A17" s="10"/>
       <c r="B17" s="15"/>
-      <c r="I17" s="20"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="A18" s="10"/>
       <c r="B18" s="15"/>
-      <c r="I18" s="20"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="A19" s="10"/>
       <c r="B19" s="15"/>
-      <c r="I19" s="20"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="A20" s="10"/>
       <c r="B20" s="15"/>
-      <c r="I20" s="20"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
-        <v>21</v>
-      </c>
+      <c r="A21" s="10"/>
       <c r="B21" s="15"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="A22" s="10"/>
       <c r="B22" s="15"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="A23" s="10"/>
       <c r="B23" s="15"/>
-      <c r="I23" s="20"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="A24" s="10"/>
       <c r="B24" s="15"/>
-      <c r="I24" s="20"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A25" s="10"/>
       <c r="B25" s="15"/>
-      <c r="I25" s="20"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="A26" s="10"/>
       <c r="B26" s="15"/>
-      <c r="I26" s="20"/>
+      <c r="I26" s="18"/>
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="A27" s="10"/>
       <c r="B27" s="15"/>
-      <c r="I27" s="20"/>
+      <c r="I27" s="18"/>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>28</v>
-      </c>
+      <c r="A28" s="10"/>
       <c r="B28" s="15"/>
-      <c r="I28" s="20"/>
+      <c r="I28" s="18"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
-        <v>29</v>
-      </c>
+      <c r="A29" s="10"/>
       <c r="B29" s="15"/>
-      <c r="I29" s="20"/>
+      <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="A30" s="10"/>
       <c r="B30" s="15"/>
-      <c r="I30" s="20"/>
+      <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
-        <v>31</v>
-      </c>
+      <c r="A31" s="10"/>
       <c r="B31" s="15"/>
-      <c r="I31" s="20"/>
+      <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="A32" s="10"/>
       <c r="B32" s="15"/>
-      <c r="I32" s="20"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="A33" s="10"/>
       <c r="B33" s="15"/>
-      <c r="I33" s="20"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
-        <v>34</v>
-      </c>
+      <c r="A34" s="10"/>
       <c r="B34" s="15"/>
-      <c r="I34" s="20"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="20" t="s">
-        <v>35</v>
-      </c>
+      <c r="A35" s="10"/>
       <c r="B35" s="15"/>
-      <c r="I35" s="20"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="20" t="s">
-        <v>36</v>
-      </c>
+      <c r="A36" s="10"/>
       <c r="B36" s="15"/>
-      <c r="I36" s="20"/>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
-        <v>37</v>
-      </c>
+      <c r="A37" s="10"/>
       <c r="B37" s="15"/>
-      <c r="I37" s="20"/>
+      <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="20" t="s">
-        <v>38</v>
-      </c>
+      <c r="A38" s="10"/>
       <c r="B38" s="15"/>
-      <c r="I38" s="20"/>
+      <c r="I38" s="18"/>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
-        <v>39</v>
-      </c>
+      <c r="A39" s="10"/>
       <c r="B39" s="15"/>
-      <c r="I39" s="20"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="A40" s="10"/>
       <c r="B40" s="15"/>
-      <c r="I40" s="20"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="20" t="s">
-        <v>41</v>
-      </c>
+      <c r="A41" s="10"/>
       <c r="B41" s="15"/>
-      <c r="I41" s="20"/>
+      <c r="I41" s="18"/>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
-        <v>42</v>
-      </c>
+      <c r="A42" s="10"/>
       <c r="B42" s="15"/>
-      <c r="I42" s="20"/>
+      <c r="I42" s="18"/>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="20" t="s">
-        <v>43</v>
-      </c>
+      <c r="A43" s="10"/>
       <c r="B43" s="15"/>
-      <c r="I43" s="20"/>
+      <c r="I43" s="18"/>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="20" t="s">
-        <v>44</v>
-      </c>
+      <c r="A44" s="10"/>
       <c r="B44" s="15"/>
-      <c r="I44" s="20"/>
+      <c r="I44" s="18"/>
     </row>
     <row r="45" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="20" t="s">
-        <v>45</v>
-      </c>
+      <c r="A45" s="10"/>
       <c r="B45" s="15"/>
-      <c r="I45" s="20"/>
+      <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="20" t="s">
-        <v>46</v>
-      </c>
+      <c r="A46" s="10"/>
       <c r="B46" s="15"/>
-      <c r="I46" s="20"/>
+      <c r="I46" s="18"/>
     </row>
     <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="A47" s="10"/>
       <c r="B47" s="15"/>
-      <c r="I47" s="20"/>
+      <c r="I47" s="18"/>
     </row>
     <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="A48" s="10"/>
       <c r="B48" s="15"/>
-      <c r="I48" s="20"/>
+      <c r="I48" s="18"/>
     </row>
     <row r="49" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="20" t="s">
-        <v>49</v>
-      </c>
+      <c r="A49" s="10"/>
       <c r="B49" s="15"/>
-      <c r="I49" s="20"/>
+      <c r="I49" s="18"/>
     </row>
     <row r="50" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="A50" s="10"/>
       <c r="B50" s="15"/>
-      <c r="I50" s="20"/>
+      <c r="I50" s="18"/>
     </row>
     <row r="51" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
-        <v>51</v>
-      </c>
+      <c r="A51" s="10"/>
       <c r="B51" s="15"/>
-      <c r="I51" s="20"/>
+      <c r="I51" s="18"/>
     </row>
     <row r="52" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="20" t="s">
-        <v>52</v>
-      </c>
+      <c r="A52" s="10"/>
       <c r="B52" s="15"/>
-      <c r="I52" s="20"/>
+      <c r="I52" s="18"/>
     </row>
     <row r="53" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="20" t="s">
-        <v>53</v>
-      </c>
+      <c r="A53" s="10"/>
       <c r="B53" s="15"/>
-      <c r="I53" s="20"/>
+      <c r="I53" s="18"/>
     </row>
     <row r="54" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
-        <v>54</v>
-      </c>
+      <c r="A54" s="10"/>
       <c r="B54" s="15"/>
-      <c r="I54" s="20"/>
+      <c r="I54" s="18"/>
     </row>
     <row r="55" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="20" t="s">
-        <v>55</v>
-      </c>
+      <c r="A55" s="10"/>
       <c r="B55" s="15"/>
-      <c r="I55" s="20"/>
+      <c r="I55" s="18"/>
     </row>
     <row r="56" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="A56" s="10"/>
       <c r="B56" s="15"/>
-      <c r="I56" s="20"/>
+      <c r="I56" s="18"/>
     </row>
     <row r="57" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="20" t="s">
-        <v>57</v>
-      </c>
+      <c r="A57" s="10"/>
       <c r="B57" s="15"/>
-      <c r="I57" s="20"/>
+      <c r="I57" s="18"/>
     </row>
     <row r="58" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="20" t="s">
-        <v>58</v>
-      </c>
+      <c r="A58" s="10"/>
       <c r="B58" s="15"/>
-      <c r="I58" s="20"/>
+      <c r="I58" s="18"/>
     </row>
     <row r="59" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="20" t="s">
-        <v>4</v>
-      </c>
+      <c r="A59" s="10"/>
       <c r="B59" s="15"/>
-      <c r="I59" s="20"/>
+      <c r="I59" s="18"/>
     </row>
     <row r="60" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="20" t="s">
-        <v>59</v>
-      </c>
+      <c r="A60" s="10"/>
       <c r="B60" s="15"/>
-      <c r="I60" s="20"/>
+      <c r="I60" s="18"/>
     </row>
     <row r="61" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="A61" s="10"/>
       <c r="B61" s="15"/>
-      <c r="I61" s="20"/>
+      <c r="I61" s="18"/>
     </row>
     <row r="62" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="20" t="s">
-        <v>61</v>
-      </c>
+      <c r="A62" s="10"/>
       <c r="B62" s="15"/>
-      <c r="I62" s="20"/>
+      <c r="I62" s="18"/>
     </row>
     <row r="63" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="20" t="s">
-        <v>62</v>
-      </c>
+      <c r="A63" s="10"/>
       <c r="B63" s="15"/>
-      <c r="I63" s="20"/>
+      <c r="I63" s="18"/>
     </row>
     <row r="64" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="A64" s="10"/>
       <c r="B64" s="15"/>
-      <c r="I64" s="20"/>
+      <c r="I64" s="18"/>
     </row>
     <row r="65" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="20" t="s">
-        <v>64</v>
-      </c>
+      <c r="A65" s="10"/>
       <c r="B65" s="15"/>
-      <c r="I65" s="20"/>
+      <c r="I65" s="18"/>
     </row>
     <row r="66" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="20" t="s">
-        <v>65</v>
-      </c>
+      <c r="A66" s="10"/>
       <c r="B66" s="15"/>
-      <c r="I66" s="20"/>
+      <c r="I66" s="18"/>
     </row>
     <row r="67" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="20" t="s">
-        <v>66</v>
-      </c>
+      <c r="A67" s="10"/>
       <c r="B67" s="15"/>
-      <c r="I67" s="20"/>
+      <c r="I67" s="18"/>
     </row>
     <row r="68" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
       <c r="B68" s="15"/>
-      <c r="I68" s="20"/>
+      <c r="I68" s="18"/>
     </row>
     <row r="69" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10"/>
       <c r="B69" s="15"/>
-      <c r="I69" s="20"/>
+      <c r="I69" s="18"/>
     </row>
     <row r="70" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10"/>
       <c r="B70" s="15"/>
-      <c r="I70" s="20"/>
+      <c r="I70" s="18"/>
     </row>
     <row r="71" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="15"/>
-      <c r="I71" s="20"/>
+      <c r="I71" s="18"/>
     </row>
     <row r="72" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="10"/>
       <c r="B72" s="15"/>
-      <c r="I72" s="20"/>
+      <c r="I72" s="18"/>
     </row>
     <row r="73" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="10"/>
       <c r="B73" s="15"/>
-      <c r="I73" s="20"/>
+      <c r="I73" s="18"/>
     </row>
     <row r="74" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10"/>
       <c r="B74" s="15"/>
-      <c r="I74" s="20"/>
+      <c r="I74" s="18"/>
     </row>
     <row r="75" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10"/>
       <c r="B75" s="15"/>
-      <c r="I75" s="20"/>
+      <c r="I75" s="18"/>
     </row>
     <row r="76" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
       <c r="B76" s="15"/>
-      <c r="I76" s="20"/>
+      <c r="I76" s="18"/>
     </row>
     <row r="77" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="10"/>
       <c r="B77" s="15"/>
-      <c r="I77" s="20"/>
+      <c r="I77" s="18"/>
     </row>
     <row r="78" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10"/>
       <c r="B78" s="15"/>
-      <c r="I78" s="20"/>
+      <c r="I78" s="18"/>
     </row>
     <row r="79" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10"/>
       <c r="B79" s="15"/>
-      <c r="I79" s="20"/>
+      <c r="I79" s="18"/>
     </row>
     <row r="80" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="10"/>
       <c r="B80" s="15"/>
-      <c r="I80" s="20"/>
+      <c r="I80" s="18"/>
     </row>
     <row r="81" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="10"/>
       <c r="B81" s="15"/>
-      <c r="I81" s="20"/>
+      <c r="I81" s="18"/>
     </row>
     <row r="82" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="10"/>
       <c r="B82" s="15"/>
-      <c r="I82" s="20"/>
+      <c r="I82" s="18"/>
     </row>
     <row r="83" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="10"/>
       <c r="B83" s="15"/>
-      <c r="I83" s="20"/>
+      <c r="I83" s="18"/>
     </row>
     <row r="84" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10"/>
       <c r="B84" s="15"/>
-      <c r="I84" s="20"/>
+      <c r="I84" s="18"/>
     </row>
     <row r="85" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10"/>
       <c r="B85" s="15"/>
-      <c r="I85" s="20"/>
+      <c r="I85" s="18"/>
     </row>
     <row r="86" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="10"/>
       <c r="B86" s="15"/>
-      <c r="I86" s="20"/>
+      <c r="I86" s="18"/>
     </row>
     <row r="87" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="10"/>
       <c r="B87" s="15"/>
-      <c r="I87" s="20"/>
+      <c r="I87" s="18"/>
     </row>
     <row r="88" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="10"/>
       <c r="B88" s="15"/>
-      <c r="I88" s="20"/>
+      <c r="I88" s="18"/>
     </row>
     <row r="89" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="10"/>
       <c r="B89" s="15"/>
-      <c r="I89" s="20"/>
+      <c r="I89" s="18"/>
     </row>
     <row r="90" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="10"/>
       <c r="B90" s="15"/>
-      <c r="I90" s="20"/>
+      <c r="I90" s="18"/>
     </row>
     <row r="91" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="10"/>
       <c r="B91" s="15"/>
-      <c r="I91" s="20"/>
+      <c r="I91" s="18"/>
     </row>
     <row r="92" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="10"/>
       <c r="B92" s="15"/>
-      <c r="I92" s="20"/>
+      <c r="I92" s="18"/>
     </row>
     <row r="93" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="10"/>
       <c r="B93" s="15"/>
-      <c r="I93" s="20"/>
+      <c r="I93" s="18"/>
     </row>
     <row r="94" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="10"/>
       <c r="B94" s="15"/>
-      <c r="I94" s="20"/>
+      <c r="I94" s="18"/>
     </row>
     <row r="95" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="10"/>
       <c r="B95" s="15"/>
-      <c r="I95" s="20"/>
+      <c r="I95" s="18"/>
     </row>
     <row r="96" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="10"/>
       <c r="B96" s="15"/>
-      <c r="I96" s="20"/>
+      <c r="I96" s="18"/>
     </row>
     <row r="97" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="10"/>
       <c r="B97" s="15"/>
-      <c r="I97" s="20"/>
+      <c r="I97" s="18"/>
     </row>
     <row r="98" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="10"/>
       <c r="B98" s="15"/>
-      <c r="I98" s="20"/>
+      <c r="I98" s="18"/>
     </row>
     <row r="99" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="10"/>
       <c r="B99" s="15"/>
-      <c r="I99" s="20"/>
+      <c r="I99" s="18"/>
     </row>
     <row r="100" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="10"/>
       <c r="B100" s="15"/>
-      <c r="I100" s="20"/>
+      <c r="I100" s="18"/>
     </row>
     <row r="101" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="10"/>
       <c r="B101" s="15"/>
-      <c r="I101" s="20"/>
+      <c r="I101" s="18"/>
     </row>
     <row r="102" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="10"/>
       <c r="B102" s="15"/>
-      <c r="I102" s="20"/>
+      <c r="I102" s="18"/>
     </row>
     <row r="103" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="10"/>
       <c r="B103" s="15"/>
-      <c r="I103" s="20"/>
+      <c r="I103" s="18"/>
     </row>
     <row r="104" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="10"/>
       <c r="B104" s="15"/>
-      <c r="I104" s="20"/>
+      <c r="I104" s="18"/>
     </row>
     <row r="105" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="10"/>
       <c r="B105" s="15"/>
-      <c r="I105" s="20"/>
+      <c r="I105" s="18"/>
     </row>
     <row r="106" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="10"/>
       <c r="B106" s="15"/>
-      <c r="I106" s="20"/>
+      <c r="I106" s="18"/>
     </row>
     <row r="107" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="10"/>
       <c r="B107" s="15"/>
-      <c r="I107" s="20"/>
+      <c r="I107" s="18"/>
     </row>
     <row r="108" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="10"/>
       <c r="B108" s="15"/>
-      <c r="I108" s="20"/>
+      <c r="I108" s="18"/>
     </row>
     <row r="109" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="10"/>
       <c r="B109" s="15"/>
-      <c r="I109" s="20"/>
+      <c r="I109" s="18"/>
     </row>
     <row r="110" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="10"/>
       <c r="B110" s="15"/>
-      <c r="I110" s="20"/>
+      <c r="I110" s="18"/>
     </row>
     <row r="111" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="10"/>
       <c r="B111" s="15"/>
-      <c r="I111" s="20"/>
+      <c r="I111" s="18"/>
     </row>
     <row r="112" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="10"/>
       <c r="B112" s="15"/>
-      <c r="I112" s="20"/>
+      <c r="I112" s="18"/>
     </row>
     <row r="113" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="10"/>
       <c r="B113" s="15"/>
-      <c r="I113" s="20"/>
+      <c r="I113" s="18"/>
     </row>
     <row r="114" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="10"/>
       <c r="B114" s="15"/>
-      <c r="I114" s="20"/>
+      <c r="I114" s="18"/>
     </row>
     <row r="115" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="10"/>
       <c r="B115" s="15"/>
-      <c r="I115" s="20"/>
+      <c r="I115" s="18"/>
     </row>
     <row r="116" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="10"/>
       <c r="B116" s="15"/>
-      <c r="I116" s="20"/>
+      <c r="I116" s="18"/>
     </row>
     <row r="117" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="10"/>
       <c r="B117" s="15"/>
-      <c r="I117" s="20"/>
+      <c r="I117" s="18"/>
     </row>
     <row r="118" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="10"/>
       <c r="B118" s="15"/>
-      <c r="I118" s="20"/>
+      <c r="I118" s="18"/>
     </row>
     <row r="119" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="10"/>
       <c r="B119" s="15"/>
-      <c r="I119" s="20"/>
+      <c r="I119" s="18"/>
     </row>
     <row r="120" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="10"/>
       <c r="B120" s="15"/>
-      <c r="I120" s="20"/>
+      <c r="I120" s="18"/>
     </row>
     <row r="121" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="10"/>
       <c r="B121" s="15"/>
-      <c r="I121" s="20"/>
+      <c r="I121" s="18"/>
     </row>
     <row r="122" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="10"/>
       <c r="B122" s="15"/>
-      <c r="I122" s="20"/>
+      <c r="I122" s="18"/>
     </row>
     <row r="123" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="10"/>
       <c r="B123" s="15"/>
-      <c r="I123" s="20"/>
+      <c r="I123" s="18"/>
     </row>
     <row r="124" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="10"/>
       <c r="B124" s="15"/>
-      <c r="I124" s="20"/>
+      <c r="I124" s="18"/>
     </row>
     <row r="125" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10"/>
       <c r="B125" s="15"/>
-      <c r="I125" s="20"/>
+      <c r="I125" s="18"/>
     </row>
     <row r="126" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="10"/>
       <c r="B126" s="15"/>
-      <c r="I126" s="20"/>
+      <c r="I126" s="18"/>
     </row>
     <row r="127" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="10"/>
       <c r="B127" s="15"/>
-      <c r="I127" s="20"/>
+      <c r="I127" s="18"/>
     </row>
     <row r="128" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="10"/>
       <c r="B128" s="15"/>
-      <c r="I128" s="20"/>
+      <c r="I128" s="18"/>
     </row>
     <row r="129" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="10"/>
       <c r="B129" s="15"/>
-      <c r="I129" s="20"/>
+      <c r="I129" s="18"/>
     </row>
     <row r="130" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="10"/>
       <c r="B130" s="15"/>
-      <c r="I130" s="20"/>
+      <c r="I130" s="18"/>
     </row>
     <row r="131" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="10"/>
       <c r="B131" s="15"/>
-      <c r="I131" s="20"/>
+      <c r="I131" s="18"/>
     </row>
     <row r="132" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="10"/>
       <c r="B132" s="15"/>
-      <c r="I132" s="20"/>
+      <c r="I132" s="18"/>
     </row>
     <row r="133" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="10"/>
       <c r="B133" s="15"/>
-      <c r="I133" s="20"/>
+      <c r="I133" s="18"/>
     </row>
     <row r="134" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="10"/>
       <c r="B134" s="15"/>
-      <c r="I134" s="20"/>
+      <c r="I134" s="18"/>
     </row>
     <row r="135" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="10"/>
       <c r="B135" s="15"/>
-      <c r="I135" s="20"/>
+      <c r="I135" s="18"/>
     </row>
     <row r="136" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="10"/>
       <c r="B136" s="15"/>
-      <c r="I136" s="20"/>
+      <c r="I136" s="18"/>
     </row>
     <row r="137" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="10"/>
       <c r="B137" s="15"/>
-      <c r="I137" s="20"/>
+      <c r="I137" s="18"/>
     </row>
     <row r="138" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="10"/>
       <c r="B138" s="15"/>
-      <c r="I138" s="20"/>
+      <c r="I138" s="18"/>
     </row>
     <row r="139" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="10"/>
       <c r="B139" s="15"/>
-      <c r="I139" s="20"/>
+      <c r="I139" s="18"/>
     </row>
     <row r="140" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="10"/>
       <c r="B140" s="15"/>
-      <c r="I140" s="20"/>
+      <c r="I140" s="18"/>
     </row>
     <row r="141" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="10"/>
       <c r="B141" s="15"/>
-      <c r="I141" s="20"/>
+      <c r="I141" s="18"/>
     </row>
     <row r="142" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="10"/>
       <c r="B142" s="15"/>
-      <c r="I142" s="20"/>
+      <c r="I142" s="18"/>
     </row>
     <row r="143" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="10"/>
       <c r="B143" s="15"/>
-      <c r="I143" s="20"/>
+      <c r="I143" s="18"/>
     </row>
     <row r="144" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="10"/>
       <c r="B144" s="15"/>
-      <c r="I144" s="20"/>
+      <c r="I144" s="18"/>
     </row>
     <row r="145" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="10"/>
       <c r="B145" s="15"/>
-      <c r="I145" s="20"/>
+      <c r="I145" s="18"/>
     </row>
     <row r="146" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="10"/>
       <c r="B146" s="15"/>
-      <c r="I146" s="20"/>
+      <c r="I146" s="18"/>
     </row>
     <row r="147" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="10"/>
       <c r="B147" s="15"/>
-      <c r="I147" s="20"/>
+      <c r="I147" s="18"/>
     </row>
     <row r="148" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="10"/>
       <c r="B148" s="15"/>
-      <c r="I148" s="20"/>
+      <c r="I148" s="18"/>
     </row>
     <row r="149" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="10"/>
       <c r="B149" s="15"/>
-      <c r="I149" s="20"/>
+      <c r="I149" s="18"/>
     </row>
     <row r="150" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="10"/>
       <c r="B150" s="15"/>
-      <c r="I150" s="20"/>
+      <c r="I150" s="18"/>
     </row>
     <row r="151" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="10"/>
       <c r="B151" s="15"/>
-      <c r="I151" s="20"/>
+      <c r="I151" s="18"/>
     </row>
     <row r="152" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="10"/>
       <c r="B152" s="15"/>
-      <c r="I152" s="20"/>
+      <c r="I152" s="18"/>
     </row>
     <row r="153" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="10"/>
       <c r="B153" s="15"/>
-      <c r="I153" s="20"/>
+      <c r="I153" s="18"/>
     </row>
     <row r="154" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="10"/>
       <c r="B154" s="15"/>
-      <c r="I154" s="20"/>
+      <c r="I154" s="18"/>
     </row>
     <row r="155" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="10"/>
       <c r="B155" s="15"/>
-      <c r="I155" s="20"/>
+      <c r="I155" s="18"/>
     </row>
     <row r="156" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="10"/>
       <c r="B156" s="15"/>
-      <c r="I156" s="20"/>
+      <c r="I156" s="18"/>
     </row>
     <row r="157" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="10"/>
       <c r="B157" s="15"/>
-      <c r="I157" s="20"/>
+      <c r="I157" s="18"/>
     </row>
     <row r="158" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="10"/>
       <c r="B158" s="15"/>
-      <c r="I158" s="20"/>
+      <c r="I158" s="18"/>
     </row>
     <row r="159" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="10"/>
       <c r="B159" s="15"/>
-      <c r="I159" s="20"/>
+      <c r="I159" s="18"/>
     </row>
     <row r="160" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="10"/>
       <c r="B160" s="15"/>
-      <c r="I160" s="20"/>
+      <c r="I160" s="18"/>
     </row>
     <row r="161" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="10"/>
       <c r="B161" s="15"/>
-      <c r="I161" s="20"/>
+      <c r="I161" s="18"/>
     </row>
     <row r="162" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="10"/>
       <c r="B162" s="15"/>
-      <c r="I162" s="20"/>
+      <c r="I162" s="18"/>
     </row>
     <row r="163" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="10"/>
       <c r="B163" s="15"/>
-      <c r="I163" s="20"/>
+      <c r="I163" s="18"/>
     </row>
     <row r="164" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="10"/>
       <c r="B164" s="15"/>
-      <c r="I164" s="20"/>
+      <c r="I164" s="18"/>
     </row>
     <row r="165" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="10"/>
       <c r="B165" s="15"/>
-      <c r="I165" s="20"/>
+      <c r="I165" s="18"/>
     </row>
     <row r="166" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="10"/>
       <c r="B166" s="15"/>
-      <c r="I166" s="20"/>
+      <c r="I166" s="18"/>
     </row>
     <row r="167" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="10"/>
       <c r="B167" s="15"/>
-      <c r="I167" s="20"/>
+      <c r="I167" s="18"/>
     </row>
     <row r="168" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="10"/>
       <c r="B168" s="15"/>
-      <c r="I168" s="20"/>
+      <c r="I168" s="18"/>
     </row>
     <row r="169" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="10"/>
       <c r="B169" s="15"/>
-      <c r="I169" s="20"/>
+      <c r="I169" s="18"/>
     </row>
     <row r="170" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="10"/>
       <c r="B170" s="15"/>
-      <c r="I170" s="20"/>
+      <c r="I170" s="18"/>
     </row>
     <row r="171" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="10"/>
       <c r="B171" s="15"/>
-      <c r="I171" s="20"/>
+      <c r="I171" s="18"/>
     </row>
     <row r="172" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="10"/>
       <c r="B172" s="15"/>
-      <c r="I172" s="20"/>
+      <c r="I172" s="18"/>
     </row>
     <row r="173" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="10"/>
       <c r="B173" s="15"/>
-      <c r="I173" s="20"/>
+      <c r="I173" s="18"/>
     </row>
     <row r="174" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="10"/>
       <c r="B174" s="15"/>
-      <c r="I174" s="20"/>
+      <c r="I174" s="18"/>
     </row>
     <row r="175" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="10"/>
       <c r="B175" s="15"/>
-      <c r="I175" s="20"/>
+      <c r="I175" s="18"/>
     </row>
     <row r="176" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="10"/>
       <c r="B176" s="15"/>
-      <c r="I176" s="20"/>
+      <c r="I176" s="18"/>
     </row>
     <row r="177" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="10"/>
       <c r="B177" s="15"/>
-      <c r="I177" s="20"/>
+      <c r="I177" s="18"/>
     </row>
     <row r="178" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="10"/>
       <c r="B178" s="15"/>
-      <c r="I178" s="20"/>
+      <c r="I178" s="18"/>
     </row>
     <row r="179" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="10"/>
       <c r="B179" s="15"/>
-      <c r="I179" s="20"/>
+      <c r="I179" s="18"/>
     </row>
     <row r="180" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="10"/>
       <c r="B180" s="15"/>
-      <c r="I180" s="20"/>
+      <c r="I180" s="18"/>
     </row>
     <row r="181" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="10"/>
       <c r="B181" s="15"/>
-      <c r="I181" s="20"/>
+      <c r="I181" s="18"/>
     </row>
     <row r="182" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="10"/>
       <c r="B182" s="15"/>
-      <c r="I182" s="20"/>
+      <c r="I182" s="18"/>
     </row>
     <row r="183" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="10"/>
       <c r="B183" s="15"/>
-      <c r="I183" s="20"/>
+      <c r="I183" s="18"/>
     </row>
     <row r="184" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="10"/>
       <c r="B184" s="15"/>
-      <c r="I184" s="20"/>
+      <c r="I184" s="18"/>
     </row>
     <row r="185" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="10"/>
       <c r="B185" s="15"/>
-      <c r="I185" s="20"/>
+      <c r="I185" s="18"/>
     </row>
     <row r="186" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="10"/>
       <c r="B186" s="15"/>
-      <c r="I186" s="20"/>
+      <c r="I186" s="18"/>
     </row>
     <row r="187" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="10"/>
       <c r="B187" s="15"/>
-      <c r="I187" s="20"/>
+      <c r="I187" s="18"/>
     </row>
     <row r="188" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="10"/>
       <c r="B188" s="15"/>
-      <c r="I188" s="20"/>
+      <c r="I188" s="18"/>
     </row>
     <row r="189" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="10"/>
       <c r="B189" s="15"/>
-      <c r="I189" s="20"/>
+      <c r="I189" s="18"/>
     </row>
     <row r="190" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="10"/>
       <c r="B190" s="15"/>
-      <c r="I190" s="20"/>
+      <c r="I190" s="18"/>
     </row>
     <row r="191" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="10"/>
       <c r="B191" s="15"/>
-      <c r="I191" s="20"/>
+      <c r="I191" s="18"/>
     </row>
     <row r="192" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="10"/>
       <c r="B192" s="15"/>
-      <c r="I192" s="20"/>
+      <c r="I192" s="18"/>
     </row>
     <row r="193" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="10"/>
       <c r="B193" s="15"/>
-      <c r="I193" s="20"/>
+      <c r="I193" s="18"/>
     </row>
     <row r="194" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="10"/>
       <c r="B194" s="15"/>
-      <c r="I194" s="20"/>
+      <c r="I194" s="18"/>
     </row>
     <row r="195" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="10"/>
       <c r="B195" s="15"/>
-      <c r="I195" s="20"/>
+      <c r="I195" s="18"/>
     </row>
     <row r="196" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="10"/>
       <c r="B196" s="15"/>
-      <c r="I196" s="20"/>
+      <c r="I196" s="18"/>
     </row>
     <row r="197" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="10"/>
       <c r="B197" s="15"/>
-      <c r="I197" s="20"/>
+      <c r="I197" s="18"/>
     </row>
     <row r="198" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="10"/>
       <c r="B198" s="15"/>
-      <c r="I198" s="20"/>
+      <c r="I198" s="18"/>
     </row>
     <row r="199" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="10"/>
       <c r="B199" s="15"/>
-      <c r="I199" s="20"/>
+      <c r="I199" s="18"/>
     </row>
     <row r="200" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="10"/>
       <c r="B200" s="15"/>
-      <c r="I200" s="20"/>
+      <c r="I200" s="18"/>
     </row>
     <row r="201" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="10"/>
       <c r="B201" s="15"/>
-      <c r="I201" s="20"/>
+      <c r="I201" s="18"/>
     </row>
     <row r="202" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="10"/>
       <c r="B202" s="15"/>
-      <c r="I202" s="20"/>
+      <c r="I202" s="18"/>
     </row>
     <row r="203" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="10"/>
       <c r="B203" s="15"/>
-      <c r="I203" s="20"/>
+      <c r="I203" s="18"/>
     </row>
     <row r="204" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="10"/>
       <c r="B204" s="15"/>
-      <c r="I204" s="20"/>
+      <c r="I204" s="18"/>
     </row>
     <row r="205" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="10"/>
       <c r="B205" s="15"/>
-      <c r="I205" s="20"/>
+      <c r="I205" s="18"/>
     </row>
     <row r="206" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="10"/>
       <c r="B206" s="15"/>
-      <c r="I206" s="20"/>
+      <c r="I206" s="18"/>
     </row>
     <row r="207" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="10"/>
       <c r="B207" s="15"/>
-      <c r="I207" s="20"/>
+      <c r="I207" s="18"/>
     </row>
     <row r="208" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="10"/>
       <c r="B208" s="15"/>
-      <c r="I208" s="20"/>
+      <c r="I208" s="18"/>
     </row>
     <row r="209" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="10"/>
       <c r="B209" s="15"/>
-      <c r="I209" s="20"/>
+      <c r="I209" s="18"/>
     </row>
     <row r="210" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="10"/>
       <c r="B210" s="15"/>
-      <c r="I210" s="20"/>
+      <c r="I210" s="18"/>
     </row>
     <row r="211" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="10"/>
       <c r="B211" s="15"/>
-      <c r="I211" s="20"/>
+      <c r="I211" s="18"/>
     </row>
     <row r="212" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="10"/>
       <c r="B212" s="15"/>
-      <c r="I212" s="20"/>
+      <c r="I212" s="18"/>
     </row>
     <row r="213" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="10"/>
       <c r="B213" s="15"/>
-      <c r="I213" s="20"/>
+      <c r="I213" s="18"/>
     </row>
     <row r="214" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="10"/>
       <c r="B214" s="15"/>
-      <c r="I214" s="20"/>
+      <c r="I214" s="18"/>
     </row>
     <row r="215" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="10"/>
       <c r="B215" s="15"/>
-      <c r="I215" s="20"/>
+      <c r="I215" s="18"/>
     </row>
     <row r="216" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="10"/>
       <c r="B216" s="15"/>
-      <c r="I216" s="20"/>
+      <c r="I216" s="18"/>
     </row>
     <row r="217" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="10"/>
       <c r="B217" s="15"/>
-      <c r="I217" s="20"/>
+      <c r="I217" s="18"/>
     </row>
     <row r="218" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="10"/>
       <c r="B218" s="15"/>
-      <c r="I218" s="20"/>
+      <c r="I218" s="18"/>
     </row>
     <row r="219" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="10"/>
       <c r="B219" s="15"/>
-      <c r="I219" s="20"/>
+      <c r="I219" s="18"/>
     </row>
     <row r="220" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="10"/>
       <c r="B220" s="15"/>
-      <c r="I220" s="20"/>
+      <c r="I220" s="18"/>
     </row>
     <row r="221" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="10"/>
       <c r="B221" s="15"/>
-      <c r="I221" s="20"/>
+      <c r="I221" s="18"/>
     </row>
     <row r="222" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="10"/>
       <c r="B222" s="15"/>
-      <c r="I222" s="20"/>
+      <c r="I222" s="18"/>
     </row>
     <row r="223" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="10"/>
       <c r="B223" s="15"/>
-      <c r="I223" s="20"/>
+      <c r="I223" s="18"/>
     </row>
     <row r="224" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="10"/>
       <c r="B224" s="15"/>
-      <c r="I224" s="20"/>
+      <c r="I224" s="18"/>
     </row>
     <row r="225" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="10"/>
       <c r="B225" s="15"/>
-      <c r="I225" s="20"/>
+      <c r="I225" s="18"/>
     </row>
     <row r="226" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="10"/>
       <c r="B226" s="15"/>
-      <c r="I226" s="20"/>
+      <c r="I226" s="18"/>
     </row>
     <row r="227" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="10"/>
       <c r="B227" s="15"/>
-      <c r="I227" s="20"/>
+      <c r="I227" s="18"/>
     </row>
     <row r="228" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="10"/>
       <c r="B228" s="15"/>
-      <c r="I228" s="20"/>
+      <c r="I228" s="18"/>
     </row>
     <row r="229" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="10"/>
       <c r="B229" s="15"/>
-      <c r="I229" s="20"/>
+      <c r="I229" s="18"/>
     </row>
     <row r="230" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="10"/>
       <c r="B230" s="15"/>
-      <c r="I230" s="20"/>
+      <c r="I230" s="18"/>
     </row>
     <row r="231" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="10"/>
       <c r="B231" s="15"/>
-      <c r="I231" s="20"/>
+      <c r="I231" s="18"/>
     </row>
     <row r="232" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="10"/>
       <c r="B232" s="15"/>
-      <c r="I232" s="20"/>
+      <c r="I232" s="18"/>
     </row>
     <row r="233" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="10"/>
       <c r="B233" s="15"/>
-      <c r="I233" s="20"/>
+      <c r="I233" s="18"/>
     </row>
     <row r="234" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="10"/>
       <c r="B234" s="15"/>
-      <c r="I234" s="20"/>
+      <c r="I234" s="18"/>
     </row>
     <row r="235" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="10"/>
       <c r="B235" s="15"/>
-      <c r="I235" s="20"/>
+      <c r="I235" s="18"/>
     </row>
     <row r="236" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="10"/>
       <c r="B236" s="15"/>
-      <c r="I236" s="20"/>
+      <c r="I236" s="18"/>
     </row>
     <row r="237" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="10"/>
       <c r="B237" s="15"/>
-      <c r="I237" s="20"/>
+      <c r="I237" s="18"/>
     </row>
     <row r="238" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="10"/>
       <c r="B238" s="15"/>
-      <c r="I238" s="20"/>
+      <c r="I238" s="18"/>
     </row>
     <row r="239" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="10"/>
       <c r="B239" s="15"/>
-      <c r="I239" s="20"/>
+      <c r="I239" s="18"/>
     </row>
     <row r="240" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="10"/>
       <c r="B240" s="15"/>
-      <c r="I240" s="20"/>
+      <c r="I240" s="18"/>
     </row>
     <row r="241" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="10"/>
       <c r="B241" s="15"/>
-      <c r="I241" s="20"/>
+      <c r="I241" s="18"/>
     </row>
     <row r="242" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="10"/>
       <c r="B242" s="15"/>
-      <c r="I242" s="20"/>
+      <c r="I242" s="18"/>
     </row>
     <row r="243" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="10"/>
       <c r="B243" s="15"/>
-      <c r="I243" s="20"/>
+      <c r="I243" s="18"/>
     </row>
     <row r="244" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="10"/>
       <c r="B244" s="15"/>
-      <c r="I244" s="20"/>
+      <c r="I244" s="18"/>
     </row>
     <row r="245" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="10"/>
       <c r="B245" s="15"/>
-      <c r="I245" s="20"/>
+      <c r="I245" s="18"/>
     </row>
     <row r="246" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="10"/>
       <c r="B246" s="15"/>
-      <c r="I246" s="20"/>
+      <c r="I246" s="18"/>
     </row>
     <row r="247" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="10"/>
       <c r="B247" s="15"/>
-      <c r="I247" s="20"/>
+      <c r="I247" s="18"/>
     </row>
     <row r="248" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="10"/>
       <c r="B248" s="15"/>
-      <c r="I248" s="20"/>
+      <c r="I248" s="18"/>
     </row>
     <row r="249" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="10"/>
       <c r="B249" s="15"/>
-      <c r="I249" s="20"/>
+      <c r="I249" s="18"/>
     </row>
     <row r="250" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="10"/>
       <c r="B250" s="15"/>
-      <c r="I250" s="20"/>
+      <c r="I250" s="18"/>
     </row>
     <row r="251" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="10"/>
       <c r="B251" s="15"/>
-      <c r="I251" s="20"/>
+      <c r="I251" s="18"/>
     </row>
     <row r="252" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="10"/>
       <c r="B252" s="15"/>
-      <c r="I252" s="20"/>
+      <c r="I252" s="18"/>
     </row>
     <row r="253" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="10"/>
       <c r="B253" s="15"/>
-      <c r="I253" s="20"/>
+      <c r="I253" s="18"/>
     </row>
     <row r="254" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="10"/>
       <c r="B254" s="15"/>
-      <c r="I254" s="20"/>
+      <c r="I254" s="18"/>
     </row>
     <row r="255" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="10"/>
       <c r="B255" s="15"/>
-      <c r="I255" s="20"/>
+      <c r="I255" s="18"/>
     </row>
     <row r="256" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="10"/>
       <c r="B256" s="15"/>
-      <c r="I256" s="20"/>
+      <c r="I256" s="18"/>
     </row>
     <row r="257" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="10"/>
       <c r="B257" s="15"/>
-      <c r="I257" s="20"/>
+      <c r="I257" s="18"/>
     </row>
     <row r="258" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="10"/>
       <c r="B258" s="15"/>
-      <c r="I258" s="20"/>
+      <c r="I258" s="18"/>
     </row>
     <row r="259" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="10"/>
       <c r="B259" s="15"/>
-      <c r="I259" s="20"/>
+      <c r="I259" s="18"/>
     </row>
     <row r="260" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="10"/>
       <c r="B260" s="15"/>
-      <c r="I260" s="20"/>
+      <c r="I260" s="18"/>
     </row>
     <row r="261" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="10"/>
       <c r="B261" s="15"/>
-      <c r="I261" s="20"/>
+      <c r="I261" s="18"/>
     </row>
     <row r="262" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="10"/>
       <c r="B262" s="15"/>
-      <c r="I262" s="20"/>
+      <c r="I262" s="18"/>
     </row>
     <row r="263" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="10"/>
       <c r="B263" s="15"/>
-      <c r="I263" s="20"/>
+      <c r="I263" s="18"/>
     </row>
     <row r="264" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="10"/>
       <c r="B264" s="15"/>
-      <c r="I264" s="20"/>
+      <c r="I264" s="18"/>
     </row>
     <row r="265" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="10"/>
       <c r="B265" s="15"/>
-      <c r="I265" s="20"/>
+      <c r="I265" s="18"/>
     </row>
     <row r="266" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="10"/>
       <c r="B266" s="15"/>
-      <c r="I266" s="20"/>
+      <c r="I266" s="18"/>
     </row>
     <row r="267" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="10"/>
       <c r="B267" s="15"/>
-      <c r="I267" s="20"/>
+      <c r="I267" s="18"/>
     </row>
     <row r="268" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="10"/>
       <c r="B268" s="15"/>
-      <c r="I268" s="20"/>
+      <c r="I268" s="18"/>
     </row>
     <row r="269" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="10"/>
       <c r="B269" s="15"/>
-      <c r="I269" s="20"/>
+      <c r="I269" s="18"/>
     </row>
     <row r="270" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="10"/>
-      <c r="B270" s="15"/>
-      <c r="I270" s="20"/>
+      <c r="B270" s="2"/>
+      <c r="I270" s="18"/>
     </row>
     <row r="271" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="10"/>
-      <c r="B271" s="15"/>
-      <c r="I271" s="20"/>
+      <c r="A271" s="11"/>
+      <c r="B271" s="2"/>
+      <c r="I271" s="18"/>
     </row>
     <row r="272" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A272" s="10"/>
-      <c r="B272" s="15"/>
-      <c r="I272" s="20"/>
+      <c r="A272" s="2"/>
+      <c r="B272" s="16"/>
+      <c r="I272" s="18"/>
     </row>
     <row r="273" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A273" s="10"/>
-      <c r="B273" s="15"/>
-      <c r="I273" s="20"/>
+      <c r="A273" s="2"/>
+      <c r="B273" s="16"/>
+      <c r="I273" s="18"/>
     </row>
     <row r="274" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A274" s="10"/>
-      <c r="B274" s="15"/>
-      <c r="I274" s="20"/>
+      <c r="A274" s="2"/>
+      <c r="B274" s="16"/>
+      <c r="I274" s="18"/>
     </row>
     <row r="275" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A275" s="10"/>
-      <c r="B275" s="15"/>
-      <c r="I275" s="20"/>
+      <c r="A275" s="2"/>
+      <c r="B275" s="16"/>
+      <c r="I275" s="18"/>
     </row>
     <row r="276" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A276" s="10"/>
-      <c r="B276" s="15"/>
-      <c r="I276" s="20"/>
+      <c r="A276" s="2"/>
+      <c r="B276" s="16"/>
+      <c r="I276" s="18"/>
     </row>
     <row r="277" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A277" s="10"/>
-      <c r="B277" s="15"/>
-      <c r="I277" s="20"/>
+      <c r="A277" s="2"/>
+      <c r="B277" s="16"/>
+      <c r="I277" s="18"/>
     </row>
     <row r="278" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A278" s="10"/>
-      <c r="B278" s="15"/>
-      <c r="I278" s="20"/>
+      <c r="A278" s="2"/>
+      <c r="B278" s="16"/>
+      <c r="I278" s="18"/>
     </row>
     <row r="279" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="10"/>
-      <c r="B279" s="15"/>
-      <c r="I279" s="20"/>
+      <c r="A279" s="2"/>
+      <c r="B279" s="16"/>
+      <c r="I279" s="18"/>
     </row>
     <row r="280" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A280" s="10"/>
-      <c r="B280" s="15"/>
-      <c r="I280" s="20"/>
+      <c r="A280" s="2"/>
+      <c r="B280" s="16"/>
+      <c r="I280" s="18"/>
     </row>
     <row r="281" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A281" s="10"/>
-      <c r="B281" s="15"/>
-      <c r="I281" s="20"/>
+      <c r="A281" s="2"/>
+      <c r="B281" s="16"/>
+      <c r="I281" s="18"/>
     </row>
     <row r="282" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A282" s="10"/>
-      <c r="B282" s="15"/>
-      <c r="I282" s="20"/>
+      <c r="A282" s="2"/>
+      <c r="B282" s="16"/>
+      <c r="I282" s="18"/>
     </row>
     <row r="283" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A283" s="10"/>
-      <c r="B283" s="15"/>
-      <c r="I283" s="20"/>
+      <c r="A283" s="2"/>
+      <c r="B283" s="16"/>
+      <c r="I283" s="18"/>
     </row>
     <row r="284" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="10"/>
-      <c r="B284" s="15"/>
-      <c r="I284" s="20"/>
+      <c r="A284" s="2"/>
+      <c r="B284" s="16"/>
+      <c r="I284" s="18"/>
     </row>
     <row r="285" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A285" s="10"/>
-      <c r="B285" s="15"/>
-      <c r="I285" s="20"/>
+      <c r="A285" s="2"/>
+      <c r="B285" s="16"/>
+      <c r="I285" s="18"/>
     </row>
     <row r="286" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A286" s="10"/>
-      <c r="B286" s="15"/>
-      <c r="I286" s="20"/>
+      <c r="A286" s="2"/>
+      <c r="B286" s="16"/>
+      <c r="I286" s="18"/>
     </row>
     <row r="287" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A287" s="10"/>
-      <c r="B287" s="15"/>
-      <c r="I287" s="20"/>
+      <c r="A287" s="2"/>
+      <c r="B287" s="16"/>
+      <c r="I287" s="18"/>
     </row>
     <row r="288" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A288" s="10"/>
-      <c r="B288" s="15"/>
-      <c r="I288" s="20"/>
+      <c r="A288" s="2"/>
+      <c r="B288" s="16"/>
+      <c r="I288" s="18"/>
     </row>
     <row r="289" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A289" s="10"/>
-      <c r="B289" s="15"/>
-      <c r="I289" s="20"/>
+      <c r="A289" s="2"/>
+      <c r="B289" s="16"/>
+      <c r="I289" s="18"/>
     </row>
     <row r="290" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A290" s="10"/>
-      <c r="B290" s="15"/>
-      <c r="I290" s="20"/>
+      <c r="A290" s="2"/>
+      <c r="B290" s="16"/>
+      <c r="I290" s="18"/>
     </row>
     <row r="291" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A291" s="10"/>
-      <c r="B291" s="15"/>
-      <c r="I291" s="20"/>
+      <c r="A291" s="2"/>
+      <c r="B291" s="16"/>
+      <c r="I291" s="18"/>
     </row>
     <row r="292" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="10"/>
-      <c r="B292" s="15"/>
-      <c r="I292" s="20"/>
+      <c r="A292" s="2"/>
+      <c r="B292" s="16"/>
+      <c r="I292" s="18"/>
     </row>
     <row r="293" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A293" s="10"/>
-      <c r="B293" s="15"/>
-      <c r="I293" s="20"/>
+      <c r="A293" s="2"/>
+      <c r="B293" s="16"/>
+      <c r="I293" s="18"/>
     </row>
     <row r="294" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A294" s="10"/>
-      <c r="B294" s="15"/>
-      <c r="I294" s="20"/>
+      <c r="A294" s="2"/>
+      <c r="B294" s="16"/>
+      <c r="I294" s="18"/>
     </row>
     <row r="295" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A295" s="10"/>
-      <c r="B295" s="15"/>
-      <c r="I295" s="20"/>
+      <c r="A295" s="2"/>
+      <c r="B295" s="16"/>
+      <c r="I295" s="18"/>
     </row>
     <row r="296" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A296" s="10"/>
-      <c r="B296" s="15"/>
-      <c r="I296" s="20"/>
+      <c r="A296" s="2"/>
+      <c r="B296" s="16"/>
+      <c r="I296" s="18"/>
     </row>
     <row r="297" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A297" s="10"/>
-      <c r="B297" s="15"/>
-      <c r="I297" s="20"/>
+      <c r="A297" s="2"/>
+      <c r="B297" s="16"/>
+      <c r="I297" s="18"/>
     </row>
     <row r="298" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A298" s="10"/>
-      <c r="B298" s="15"/>
-      <c r="I298" s="20"/>
+      <c r="A298" s="2"/>
+      <c r="B298" s="16"/>
+      <c r="I298" s="18"/>
     </row>
     <row r="299" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A299" s="10"/>
-      <c r="B299" s="15"/>
-      <c r="I299" s="20"/>
+      <c r="A299" s="2"/>
+      <c r="B299" s="16"/>
+      <c r="I299" s="18"/>
     </row>
     <row r="300" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A300" s="10"/>
-      <c r="B300" s="15"/>
-      <c r="I300" s="20"/>
+      <c r="A300" s="2"/>
+      <c r="B300" s="16"/>
+      <c r="I300" s="18"/>
     </row>
     <row r="301" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A301" s="10"/>
-      <c r="B301" s="15"/>
-      <c r="I301" s="20"/>
+      <c r="A301" s="2"/>
+      <c r="B301" s="16"/>
+      <c r="I301" s="18"/>
     </row>
     <row r="302" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A302" s="10"/>
-      <c r="B302" s="15"/>
-      <c r="I302" s="20"/>
+      <c r="A302" s="2"/>
+      <c r="B302" s="16"/>
+      <c r="I302" s="18"/>
     </row>
     <row r="303" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A303" s="10"/>
-      <c r="B303" s="15"/>
-      <c r="I303" s="20"/>
+      <c r="A303" s="2"/>
+      <c r="B303" s="16"/>
+      <c r="I303" s="18"/>
     </row>
     <row r="304" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A304" s="10"/>
-      <c r="B304" s="15"/>
-      <c r="I304" s="20"/>
+      <c r="A304" s="2"/>
+      <c r="B304" s="16"/>
+      <c r="I304" s="18"/>
     </row>
     <row r="305" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A305" s="10"/>
-      <c r="B305" s="15"/>
-      <c r="I305" s="20"/>
+      <c r="A305" s="2"/>
+      <c r="B305" s="16"/>
+      <c r="I305" s="18"/>
     </row>
     <row r="306" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A306" s="10"/>
-      <c r="B306" s="15"/>
-      <c r="I306" s="20"/>
+      <c r="A306" s="2"/>
+      <c r="B306" s="16"/>
+      <c r="I306" s="18"/>
     </row>
     <row r="307" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A307" s="10"/>
-      <c r="B307" s="15"/>
-      <c r="I307" s="20"/>
+      <c r="A307" s="2"/>
+      <c r="B307" s="16"/>
+      <c r="I307" s="18"/>
     </row>
     <row r="308" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A308" s="10"/>
-      <c r="B308" s="15"/>
-      <c r="I308" s="20"/>
+      <c r="A308" s="2"/>
+      <c r="B308" s="16"/>
+      <c r="I308" s="18"/>
     </row>
     <row r="309" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A309" s="10"/>
-      <c r="B309" s="15"/>
-      <c r="I309" s="20"/>
+      <c r="A309" s="2"/>
+      <c r="B309" s="16"/>
+      <c r="I309" s="18"/>
     </row>
     <row r="310" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A310" s="10"/>
-      <c r="B310" s="15"/>
-      <c r="I310" s="20"/>
+      <c r="A310" s="2"/>
+      <c r="B310" s="16"/>
+      <c r="I310" s="18"/>
     </row>
     <row r="311" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A311" s="10"/>
-      <c r="B311" s="15"/>
-      <c r="I311" s="20"/>
+      <c r="A311" s="2"/>
+      <c r="B311" s="16"/>
+      <c r="I311" s="18"/>
     </row>
     <row r="312" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A312" s="10"/>
-      <c r="B312" s="15"/>
-      <c r="I312" s="20"/>
+      <c r="A312" s="2"/>
+      <c r="B312" s="16"/>
+      <c r="I312" s="18"/>
     </row>
     <row r="313" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A313" s="10"/>
-      <c r="B313" s="15"/>
-      <c r="I313" s="20"/>
+      <c r="A313" s="2"/>
+      <c r="B313" s="16"/>
+      <c r="I313" s="18"/>
     </row>
     <row r="314" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A314" s="10"/>
-      <c r="B314" s="15"/>
-      <c r="I314" s="20"/>
+      <c r="A314" s="2"/>
+      <c r="B314" s="16"/>
+      <c r="I314" s="18"/>
     </row>
     <row r="315" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A315" s="10"/>
-      <c r="B315" s="15"/>
-      <c r="I315" s="20"/>
+      <c r="A315" s="2"/>
+      <c r="B315" s="16"/>
+      <c r="I315" s="18"/>
     </row>
     <row r="316" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A316" s="10"/>
-      <c r="B316" s="15"/>
-      <c r="I316" s="20"/>
+      <c r="A316" s="2"/>
+      <c r="B316" s="16"/>
+      <c r="I316" s="18"/>
     </row>
     <row r="317" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A317" s="10"/>
-      <c r="B317" s="15"/>
-      <c r="I317" s="20"/>
+      <c r="A317" s="2"/>
+      <c r="B317" s="16"/>
+      <c r="I317" s="18"/>
     </row>
     <row r="318" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A318" s="10"/>
-      <c r="B318" s="15"/>
-      <c r="I318" s="20"/>
+      <c r="A318" s="2"/>
+      <c r="B318" s="16"/>
+      <c r="I318" s="18"/>
     </row>
     <row r="319" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A319" s="10"/>
-      <c r="B319" s="15"/>
-      <c r="I319" s="20"/>
+      <c r="A319" s="2"/>
+      <c r="B319" s="16"/>
+      <c r="I319" s="18"/>
     </row>
     <row r="320" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A320" s="10"/>
-      <c r="B320" s="15"/>
-      <c r="I320" s="20"/>
+      <c r="A320" s="2"/>
+      <c r="B320" s="16"/>
+      <c r="I320" s="18"/>
     </row>
     <row r="321" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A321" s="10"/>
-      <c r="B321" s="15"/>
-      <c r="I321" s="20"/>
+      <c r="A321" s="2"/>
+      <c r="B321" s="16"/>
+      <c r="I321" s="18"/>
     </row>
     <row r="322" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A322" s="10"/>
-      <c r="B322" s="15"/>
-      <c r="I322" s="20"/>
+      <c r="A322" s="2"/>
+      <c r="B322" s="16"/>
+      <c r="I322" s="18"/>
     </row>
     <row r="323" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A323" s="10"/>
-      <c r="B323" s="15"/>
-      <c r="I323" s="20"/>
+      <c r="A323" s="2"/>
+      <c r="B323" s="16"/>
+      <c r="I323" s="18"/>
     </row>
     <row r="324" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A324" s="10"/>
-      <c r="B324" s="15"/>
-      <c r="I324" s="20"/>
+      <c r="A324" s="2"/>
+      <c r="B324" s="16"/>
+      <c r="I324" s="18"/>
     </row>
     <row r="325" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A325" s="10"/>
-      <c r="B325" s="15"/>
-      <c r="I325" s="20"/>
+      <c r="A325" s="2"/>
+      <c r="B325" s="16"/>
+      <c r="I325" s="18"/>
     </row>
     <row r="326" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A326" s="10"/>
-      <c r="B326" s="15"/>
-      <c r="I326" s="20"/>
+      <c r="A326" s="2"/>
+      <c r="B326" s="16"/>
+      <c r="I326" s="18"/>
     </row>
     <row r="327" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A327" s="10"/>
-      <c r="B327" s="15"/>
-      <c r="I327" s="20"/>
+      <c r="A327" s="2"/>
+      <c r="B327" s="16"/>
+      <c r="I327" s="18"/>
     </row>
     <row r="328" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A328" s="10"/>
-      <c r="B328" s="15"/>
-      <c r="I328" s="20"/>
+      <c r="A328" s="2"/>
+      <c r="B328" s="16"/>
+      <c r="I328" s="18"/>
     </row>
     <row r="329" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A329" s="10"/>
-      <c r="B329" s="15"/>
-      <c r="I329" s="20"/>
+      <c r="A329" s="2"/>
+      <c r="B329" s="16"/>
+      <c r="I329" s="18"/>
     </row>
     <row r="330" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A330" s="10"/>
-      <c r="B330" s="15"/>
-      <c r="I330" s="20"/>
+      <c r="A330" s="2"/>
+      <c r="B330" s="16"/>
+      <c r="I330" s="18"/>
     </row>
     <row r="331" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A331" s="10"/>
-      <c r="B331" s="15"/>
-      <c r="I331" s="20"/>
+      <c r="A331" s="2"/>
+      <c r="B331" s="16"/>
+      <c r="I331" s="18"/>
     </row>
     <row r="332" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A332" s="10"/>
-      <c r="B332" s="15"/>
-      <c r="I332" s="20"/>
+      <c r="A332" s="2"/>
+      <c r="B332" s="16"/>
+      <c r="I332" s="18"/>
     </row>
     <row r="333" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A333" s="10"/>
-      <c r="B333" s="15"/>
-      <c r="I333" s="20"/>
+      <c r="A333" s="2"/>
+      <c r="B333" s="2"/>
+      <c r="I333" s="18"/>
     </row>
     <row r="334" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A334" s="10"/>
-      <c r="B334" s="15"/>
-      <c r="I334" s="20"/>
+      <c r="A334" s="2"/>
+      <c r="B334" s="16"/>
+      <c r="I334" s="18"/>
     </row>
     <row r="335" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A335" s="10"/>
-      <c r="B335" s="15"/>
-      <c r="I335" s="20"/>
+      <c r="A335" s="2"/>
+      <c r="B335" s="16"/>
+      <c r="I335" s="18"/>
     </row>
     <row r="336" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A336" s="10"/>
-      <c r="B336" s="15"/>
-      <c r="I336" s="20"/>
+      <c r="A336" s="2"/>
+      <c r="B336" s="10"/>
+      <c r="I336" s="18"/>
     </row>
     <row r="337" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A337" s="10"/>
-      <c r="B337" s="15"/>
-      <c r="I337" s="20"/>
+      <c r="A337" s="12"/>
+      <c r="B337" s="2"/>
+      <c r="I337" s="18"/>
     </row>
     <row r="338" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A338" s="10"/>
-      <c r="B338" s="15"/>
-      <c r="I338" s="20"/>
+      <c r="A338" s="2"/>
+      <c r="B338" s="16"/>
+      <c r="I338" s="18"/>
     </row>
     <row r="339" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A339" s="10"/>
-      <c r="B339" s="15"/>
-      <c r="I339" s="20"/>
+      <c r="A339" s="2"/>
+      <c r="B339" s="2"/>
+      <c r="I339" s="18"/>
     </row>
     <row r="340" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A340" s="10"/>
-      <c r="B340" s="15"/>
-      <c r="I340" s="20"/>
+      <c r="A340" s="11"/>
+      <c r="B340" s="2"/>
+      <c r="I340" s="18"/>
     </row>
     <row r="341" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A341" s="10"/>
-      <c r="B341" s="15"/>
-      <c r="I341" s="20"/>
+      <c r="A341" s="13"/>
+      <c r="B341" s="2"/>
+      <c r="I341" s="18"/>
     </row>
     <row r="342" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A342" s="10"/>
-      <c r="B342" s="15"/>
-      <c r="I342" s="20"/>
+      <c r="A342" s="2"/>
+      <c r="B342" s="16"/>
+      <c r="I342" s="18"/>
     </row>
     <row r="343" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A343" s="10"/>
-      <c r="B343" s="15"/>
-      <c r="I343" s="20"/>
+      <c r="A343" s="2"/>
+      <c r="B343" s="16"/>
+      <c r="I343" s="18"/>
     </row>
     <row r="344" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A344" s="10"/>
-      <c r="B344" s="15"/>
-      <c r="I344" s="20"/>
+      <c r="A344" s="2"/>
+      <c r="B344" s="16"/>
+      <c r="I344" s="18"/>
     </row>
     <row r="345" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A345" s="10"/>
-      <c r="B345" s="15"/>
-      <c r="I345" s="20"/>
+      <c r="A345" s="2"/>
+      <c r="B345" s="10"/>
+      <c r="I345" s="18"/>
     </row>
     <row r="346" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A346" s="10"/>
-      <c r="B346" s="15"/>
-      <c r="I346" s="20"/>
+      <c r="B346" s="16"/>
+      <c r="I346" s="18"/>
     </row>
     <row r="347" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A347" s="10"/>
-      <c r="B347" s="15"/>
-      <c r="I347" s="20"/>
+      <c r="A347" s="2"/>
+      <c r="B347" s="16"/>
+      <c r="I347" s="18"/>
     </row>
     <row r="348" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A348" s="10"/>
-      <c r="B348" s="15"/>
-      <c r="I348" s="20"/>
+      <c r="A348" s="2"/>
+      <c r="B348" s="2"/>
+      <c r="I348" s="18"/>
     </row>
     <row r="349" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A349" s="10"/>
-      <c r="B349" s="15"/>
-      <c r="I349" s="20"/>
+      <c r="A349" s="2"/>
+      <c r="B349" s="2"/>
+      <c r="I349" s="18"/>
     </row>
     <row r="350" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A350" s="10"/>
-      <c r="B350" s="15"/>
-      <c r="I350" s="20"/>
+      <c r="A350" s="2"/>
+      <c r="B350" s="16"/>
+      <c r="I350" s="18"/>
     </row>
     <row r="351" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A351" s="10"/>
-      <c r="B351" s="15"/>
-      <c r="I351" s="20"/>
+      <c r="A351" s="2"/>
+      <c r="B351" s="2"/>
+      <c r="I351" s="18"/>
     </row>
     <row r="352" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A352" s="10"/>
-      <c r="B352" s="15"/>
-      <c r="I352" s="20"/>
+      <c r="A352" s="2"/>
+      <c r="B352" s="2"/>
+      <c r="I352" s="18"/>
     </row>
     <row r="353" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A353" s="10"/>
-      <c r="B353" s="15"/>
-      <c r="I353" s="20"/>
+      <c r="A353" s="2"/>
+      <c r="B353" s="12"/>
+      <c r="I353" s="18"/>
     </row>
     <row r="354" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A354" s="10"/>
-      <c r="B354" s="15"/>
-      <c r="I354" s="20"/>
+      <c r="A354" s="2"/>
+      <c r="B354" s="16"/>
+      <c r="I354" s="18"/>
     </row>
     <row r="355" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A355" s="10"/>
-      <c r="B355" s="15"/>
-      <c r="I355" s="20"/>
+      <c r="A355" s="2"/>
+      <c r="B355" s="2"/>
+      <c r="I355" s="18"/>
     </row>
     <row r="356" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A356" s="10"/>
-      <c r="B356" s="15"/>
-      <c r="I356" s="20"/>
+      <c r="B356" s="16"/>
+      <c r="I356" s="18"/>
     </row>
     <row r="357" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A357" s="10"/>
-      <c r="B357" s="15"/>
-      <c r="I357" s="20"/>
+      <c r="A357" s="2"/>
+      <c r="B357" s="12"/>
+      <c r="I357" s="18"/>
     </row>
     <row r="358" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A358" s="10"/>
-      <c r="B358" s="15"/>
-      <c r="I358" s="20"/>
+      <c r="A358" s="13"/>
+      <c r="B358" s="12"/>
+      <c r="I358" s="18"/>
     </row>
     <row r="359" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A359" s="10"/>
-      <c r="B359" s="15"/>
-      <c r="I359" s="20"/>
+      <c r="A359" s="14"/>
+      <c r="B359" s="16"/>
+      <c r="I359" s="18"/>
     </row>
     <row r="360" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A360" s="10"/>
-      <c r="B360" s="15"/>
-      <c r="I360" s="20"/>
-    </row>
-    <row r="361" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A360" s="2"/>
+      <c r="B360" s="2"/>
+      <c r="I360" s="18"/>
+    </row>
+    <row r="361" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A361" s="10"/>
-      <c r="B361" s="15"/>
-      <c r="I361" s="20"/>
-    </row>
-    <row r="362" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A362" s="10"/>
-      <c r="B362" s="15"/>
-      <c r="I362" s="20"/>
-    </row>
-    <row r="363" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A363" s="10"/>
-      <c r="B363" s="15"/>
-      <c r="I363" s="20"/>
-    </row>
-    <row r="364" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A364" s="10"/>
-      <c r="B364" s="15"/>
-      <c r="I364" s="20"/>
-    </row>
-    <row r="365" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A365" s="10"/>
-      <c r="B365" s="15"/>
-      <c r="I365" s="20"/>
-    </row>
-    <row r="366" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A366" s="10"/>
-      <c r="B366" s="15"/>
-      <c r="I366" s="20"/>
-    </row>
-    <row r="367" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A367" s="10"/>
-      <c r="B367" s="15"/>
-      <c r="I367" s="20"/>
-    </row>
-    <row r="368" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A368" s="10"/>
-      <c r="B368" s="15"/>
-      <c r="I368" s="20"/>
-    </row>
-    <row r="369" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A369" s="10"/>
-      <c r="B369" s="15"/>
-      <c r="I369" s="20"/>
-    </row>
-    <row r="370" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A370" s="10"/>
-      <c r="B370" s="15"/>
-      <c r="I370" s="20"/>
-    </row>
-    <row r="371" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A371" s="10"/>
-      <c r="B371" s="15"/>
-      <c r="I371" s="20"/>
-    </row>
-    <row r="372" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A372" s="10"/>
-      <c r="B372" s="15"/>
-      <c r="I372" s="20"/>
-    </row>
-    <row r="373" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A373" s="10"/>
-      <c r="B373" s="15"/>
-      <c r="I373" s="20"/>
-    </row>
-    <row r="374" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A374" s="10"/>
-      <c r="B374" s="15"/>
-      <c r="I374" s="20"/>
-    </row>
-    <row r="375" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A375" s="10"/>
-      <c r="B375" s="15"/>
-      <c r="I375" s="20"/>
-    </row>
-    <row r="376" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A376" s="10"/>
-      <c r="B376" s="15"/>
-      <c r="I376" s="20"/>
-    </row>
-    <row r="377" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A377" s="10"/>
-      <c r="B377" s="15"/>
-      <c r="I377" s="20"/>
-    </row>
-    <row r="378" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A378" s="10"/>
-      <c r="B378" s="15"/>
-      <c r="I378" s="20"/>
-    </row>
-    <row r="379" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A379" s="10"/>
-      <c r="B379" s="15"/>
-      <c r="I379" s="20"/>
-    </row>
-    <row r="380" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A380" s="10"/>
-      <c r="B380" s="15"/>
-      <c r="I380" s="20"/>
-    </row>
-    <row r="381" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A381" s="10"/>
-      <c r="B381" s="15"/>
-      <c r="I381" s="20"/>
-    </row>
-    <row r="382" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A382" s="10"/>
-      <c r="B382" s="15"/>
-      <c r="I382" s="20"/>
-    </row>
-    <row r="383" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A383" s="10"/>
-      <c r="B383" s="15"/>
-      <c r="I383" s="20"/>
-    </row>
-    <row r="384" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A384" s="10"/>
-      <c r="B384" s="15"/>
-      <c r="I384" s="20"/>
-    </row>
-    <row r="385" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A385" s="10"/>
-      <c r="B385" s="15"/>
-      <c r="I385" s="20"/>
-    </row>
-    <row r="386" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A386" s="10"/>
-      <c r="B386" s="15"/>
-      <c r="I386" s="20"/>
-    </row>
-    <row r="387" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A387" s="10"/>
-      <c r="B387" s="15"/>
-      <c r="I387" s="20"/>
-    </row>
-    <row r="388" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A388" s="10"/>
-      <c r="B388" s="2"/>
-      <c r="I388" s="20"/>
-    </row>
-    <row r="389" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A389" s="11"/>
-      <c r="B389" s="2"/>
-      <c r="I389" s="20"/>
-    </row>
-    <row r="390" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A390" s="2"/>
-      <c r="B390" s="16"/>
-      <c r="I390" s="20"/>
-    </row>
-    <row r="391" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A391" s="2"/>
-      <c r="B391" s="16"/>
-      <c r="I391" s="20"/>
-    </row>
-    <row r="392" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A392" s="2"/>
-      <c r="B392" s="16"/>
-      <c r="I392" s="20"/>
-    </row>
-    <row r="393" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A393" s="2"/>
-      <c r="B393" s="16"/>
-      <c r="I393" s="20"/>
-    </row>
-    <row r="394" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A394" s="2"/>
-      <c r="B394" s="16"/>
-      <c r="I394" s="20"/>
-    </row>
-    <row r="395" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A395" s="2"/>
-      <c r="B395" s="16"/>
-      <c r="I395" s="20"/>
-    </row>
-    <row r="396" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A396" s="2"/>
-      <c r="B396" s="16"/>
-      <c r="I396" s="20"/>
-    </row>
-    <row r="397" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A397" s="2"/>
-      <c r="B397" s="16"/>
-      <c r="I397" s="20"/>
-    </row>
-    <row r="398" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A398" s="2"/>
-      <c r="B398" s="16"/>
-      <c r="I398" s="20"/>
-    </row>
-    <row r="399" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A399" s="2"/>
-      <c r="B399" s="16"/>
-      <c r="I399" s="20"/>
-    </row>
-    <row r="400" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A400" s="2"/>
-      <c r="B400" s="16"/>
-      <c r="I400" s="20"/>
-    </row>
-    <row r="401" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A401" s="2"/>
-      <c r="B401" s="16"/>
-      <c r="I401" s="20"/>
-    </row>
-    <row r="402" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A402" s="2"/>
-      <c r="B402" s="16"/>
-      <c r="I402" s="20"/>
-    </row>
-    <row r="403" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A403" s="2"/>
-      <c r="B403" s="16"/>
-      <c r="I403" s="20"/>
-    </row>
-    <row r="404" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A404" s="2"/>
-      <c r="B404" s="16"/>
-      <c r="I404" s="20"/>
-    </row>
-    <row r="405" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A405" s="2"/>
-      <c r="B405" s="16"/>
-      <c r="I405" s="20"/>
-    </row>
-    <row r="406" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A406" s="2"/>
-      <c r="B406" s="16"/>
-      <c r="I406" s="20"/>
-    </row>
-    <row r="407" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A407" s="2"/>
-      <c r="B407" s="16"/>
-      <c r="I407" s="20"/>
-    </row>
-    <row r="408" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A408" s="2"/>
-      <c r="B408" s="16"/>
-      <c r="I408" s="20"/>
-    </row>
-    <row r="409" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A409" s="2"/>
-      <c r="B409" s="16"/>
-      <c r="I409" s="20"/>
-    </row>
-    <row r="410" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A410" s="2"/>
-      <c r="B410" s="16"/>
-      <c r="I410" s="20"/>
-    </row>
-    <row r="411" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A411" s="2"/>
-      <c r="B411" s="16"/>
-      <c r="I411" s="20"/>
-    </row>
-    <row r="412" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A412" s="2"/>
-      <c r="B412" s="16"/>
-      <c r="I412" s="20"/>
-    </row>
-    <row r="413" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A413" s="2"/>
-      <c r="B413" s="16"/>
-      <c r="I413" s="20"/>
-    </row>
-    <row r="414" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A414" s="2"/>
-      <c r="B414" s="16"/>
-      <c r="I414" s="20"/>
-    </row>
-    <row r="415" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A415" s="2"/>
-      <c r="B415" s="16"/>
-      <c r="I415" s="20"/>
-    </row>
-    <row r="416" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A416" s="2"/>
-      <c r="B416" s="16"/>
-      <c r="I416" s="20"/>
-    </row>
-    <row r="417" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A417" s="2"/>
-      <c r="B417" s="16"/>
-      <c r="I417" s="20"/>
-    </row>
-    <row r="418" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A418" s="2"/>
-      <c r="B418" s="16"/>
-      <c r="I418" s="20"/>
-    </row>
-    <row r="419" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A419" s="2"/>
-      <c r="B419" s="16"/>
-      <c r="I419" s="20"/>
-    </row>
-    <row r="420" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A420" s="2"/>
-      <c r="B420" s="16"/>
-      <c r="I420" s="20"/>
-    </row>
-    <row r="421" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A421" s="2"/>
-      <c r="B421" s="16"/>
-      <c r="I421" s="20"/>
-    </row>
-    <row r="422" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A422" s="2"/>
-      <c r="B422" s="16"/>
-      <c r="I422" s="20"/>
-    </row>
-    <row r="423" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A423" s="2"/>
-      <c r="B423" s="16"/>
-      <c r="I423" s="20"/>
-    </row>
-    <row r="424" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A424" s="2"/>
-      <c r="B424" s="16"/>
-      <c r="I424" s="20"/>
-    </row>
-    <row r="425" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A425" s="2"/>
-      <c r="B425" s="16"/>
-      <c r="I425" s="20"/>
-    </row>
-    <row r="426" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A426" s="2"/>
-      <c r="B426" s="16"/>
-      <c r="I426" s="20"/>
-    </row>
-    <row r="427" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A427" s="2"/>
-      <c r="B427" s="16"/>
-      <c r="I427" s="20"/>
-    </row>
-    <row r="428" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A428" s="2"/>
-      <c r="B428" s="16"/>
-      <c r="I428" s="20"/>
-    </row>
-    <row r="429" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A429" s="2"/>
-      <c r="B429" s="16"/>
-      <c r="I429" s="20"/>
-    </row>
-    <row r="430" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A430" s="2"/>
-      <c r="B430" s="16"/>
-      <c r="I430" s="20"/>
-    </row>
-    <row r="431" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A431" s="2"/>
-      <c r="B431" s="16"/>
-      <c r="I431" s="20"/>
-    </row>
-    <row r="432" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A432" s="2"/>
-      <c r="B432" s="16"/>
-      <c r="I432" s="20"/>
-    </row>
-    <row r="433" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A433" s="2"/>
-      <c r="B433" s="16"/>
-      <c r="I433" s="20"/>
-    </row>
-    <row r="434" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A434" s="2"/>
-      <c r="B434" s="16"/>
-      <c r="I434" s="20"/>
-    </row>
-    <row r="435" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A435" s="2"/>
-      <c r="B435" s="16"/>
-      <c r="I435" s="20"/>
-    </row>
-    <row r="436" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A436" s="2"/>
-      <c r="B436" s="16"/>
-      <c r="I436" s="20"/>
-    </row>
-    <row r="437" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A437" s="2"/>
-      <c r="B437" s="16"/>
-      <c r="I437" s="20"/>
-    </row>
-    <row r="438" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A438" s="2"/>
-      <c r="B438" s="16"/>
-      <c r="I438" s="20"/>
-    </row>
-    <row r="439" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A439" s="2"/>
-      <c r="B439" s="16"/>
-      <c r="I439" s="20"/>
-    </row>
-    <row r="440" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A440" s="2"/>
-      <c r="B440" s="16"/>
-      <c r="I440" s="20"/>
-    </row>
-    <row r="441" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A441" s="2"/>
-      <c r="B441" s="16"/>
-      <c r="I441" s="20"/>
-    </row>
-    <row r="442" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A442" s="2"/>
-      <c r="B442" s="16"/>
-      <c r="I442" s="20"/>
-    </row>
-    <row r="443" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A443" s="2"/>
-      <c r="B443" s="16"/>
-      <c r="I443" s="20"/>
-    </row>
-    <row r="444" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A444" s="2"/>
-      <c r="B444" s="16"/>
-      <c r="I444" s="20"/>
-    </row>
-    <row r="445" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A445" s="2"/>
-      <c r="B445" s="16"/>
-      <c r="I445" s="20"/>
-    </row>
-    <row r="446" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A446" s="2"/>
-      <c r="B446" s="16"/>
-      <c r="I446" s="20"/>
-    </row>
-    <row r="447" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A447" s="2"/>
-      <c r="B447" s="16"/>
-      <c r="I447" s="20"/>
-    </row>
-    <row r="448" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A448" s="2"/>
-      <c r="B448" s="16"/>
-      <c r="I448" s="20"/>
-    </row>
-    <row r="449" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A449" s="2"/>
-      <c r="B449" s="16"/>
-      <c r="I449" s="20"/>
-    </row>
-    <row r="450" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A450" s="2"/>
-      <c r="B450" s="16"/>
-      <c r="I450" s="20"/>
-    </row>
-    <row r="451" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A451" s="2"/>
-      <c r="B451" s="2"/>
-      <c r="I451" s="20"/>
-    </row>
-    <row r="452" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A452" s="2"/>
-      <c r="B452" s="16"/>
-      <c r="I452" s="20"/>
-    </row>
-    <row r="453" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A453" s="2"/>
-      <c r="B453" s="16"/>
-      <c r="I453" s="20"/>
-    </row>
-    <row r="454" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A454" s="2"/>
-      <c r="B454" s="10"/>
-      <c r="I454" s="20"/>
-    </row>
-    <row r="455" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A455" s="12"/>
-      <c r="B455" s="2"/>
-      <c r="I455" s="20"/>
-    </row>
-    <row r="456" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A456" s="2"/>
-      <c r="B456" s="16"/>
-      <c r="I456" s="20"/>
-    </row>
-    <row r="457" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A457" s="2"/>
-      <c r="B457" s="2"/>
-      <c r="I457" s="20"/>
-    </row>
-    <row r="458" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A458" s="11"/>
-      <c r="B458" s="2"/>
-      <c r="I458" s="20"/>
-    </row>
-    <row r="459" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A459" s="13"/>
-      <c r="B459" s="2"/>
-      <c r="I459" s="20"/>
-    </row>
-    <row r="460" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A460" s="2"/>
-      <c r="B460" s="16"/>
-      <c r="I460" s="20"/>
-    </row>
-    <row r="461" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A461" s="2"/>
-      <c r="B461" s="16"/>
-      <c r="I461" s="20"/>
-    </row>
-    <row r="462" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A462" s="2"/>
-      <c r="B462" s="16"/>
-      <c r="I462" s="20"/>
-    </row>
-    <row r="463" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A463" s="2"/>
-      <c r="B463" s="10"/>
-      <c r="I463" s="20"/>
-    </row>
-    <row r="464" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A464" s="10"/>
-      <c r="B464" s="16"/>
-      <c r="I464" s="20"/>
-    </row>
-    <row r="465" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A465" s="2"/>
-      <c r="B465" s="16"/>
-      <c r="I465" s="20"/>
-    </row>
-    <row r="466" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A466" s="2"/>
-      <c r="B466" s="2"/>
-      <c r="I466" s="20"/>
-    </row>
-    <row r="467" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A467" s="2"/>
-      <c r="B467" s="2"/>
-      <c r="I467" s="20"/>
-    </row>
-    <row r="468" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A468" s="2"/>
-      <c r="B468" s="16"/>
-      <c r="I468" s="20"/>
-    </row>
-    <row r="469" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A469" s="2"/>
-      <c r="B469" s="2"/>
-      <c r="I469" s="20"/>
-    </row>
-    <row r="470" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A470" s="2"/>
-      <c r="B470" s="2"/>
-      <c r="I470" s="20"/>
-    </row>
-    <row r="471" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A471" s="2"/>
-      <c r="B471" s="12"/>
-      <c r="I471" s="20"/>
-    </row>
-    <row r="472" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A472" s="2"/>
-      <c r="B472" s="16"/>
-      <c r="I472" s="20"/>
-    </row>
-    <row r="473" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A473" s="2"/>
-      <c r="B473" s="2"/>
-      <c r="I473" s="20"/>
-    </row>
-    <row r="474" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A474" s="10"/>
-      <c r="B474" s="16"/>
-      <c r="I474" s="20"/>
-    </row>
-    <row r="475" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A475" s="2"/>
-      <c r="B475" s="12"/>
-      <c r="I475" s="20"/>
-    </row>
-    <row r="476" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A476" s="13"/>
-      <c r="B476" s="12"/>
-      <c r="I476" s="20"/>
-    </row>
-    <row r="477" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A477" s="14"/>
-      <c r="B477" s="16"/>
-      <c r="I477" s="20"/>
-    </row>
-    <row r="478" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A478" s="2"/>
-      <c r="B478" s="2"/>
-      <c r="I478" s="20"/>
-    </row>
-    <row r="479" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A479" s="10"/>
+      <c r="B361" s="7"/>
+    </row>
+    <row r="362" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A362" s="6"/>
+      <c r="B362" s="7"/>
+    </row>
+    <row r="363" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A363" s="6"/>
+      <c r="B363" s="7"/>
+    </row>
+    <row r="364" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A364" s="6"/>
+      <c r="B364" s="7"/>
+    </row>
+    <row r="365" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A365" s="6"/>
+      <c r="B365" s="7"/>
+    </row>
+    <row r="366" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A366" s="6"/>
+      <c r="B366" s="7"/>
+    </row>
+    <row r="367" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A367" s="6"/>
+      <c r="B367" s="7"/>
+    </row>
+    <row r="368" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A368" s="6"/>
+      <c r="B368" s="7"/>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A369" s="6"/>
+      <c r="B369" s="7"/>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A370" s="6"/>
+      <c r="B370" s="7"/>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A371" s="6"/>
+      <c r="B371" s="7"/>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A372" s="6"/>
+      <c r="B372" s="7"/>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A373" s="6"/>
+      <c r="B373" s="7"/>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A374" s="6"/>
+      <c r="B374" s="7"/>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A375" s="6"/>
+      <c r="B375" s="7"/>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A376" s="6"/>
+      <c r="B376" s="7"/>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A377" s="6"/>
+      <c r="B377" s="7"/>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A378" s="6"/>
+      <c r="B378" s="7"/>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A379" s="6"/>
+      <c r="B379" s="7"/>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A380" s="6"/>
+      <c r="B380" s="7"/>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A381" s="6"/>
+      <c r="B381" s="7"/>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A382" s="6"/>
+      <c r="B382" s="7"/>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A383" s="6"/>
+      <c r="B383" s="7"/>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A384" s="6"/>
+      <c r="B384" s="7"/>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A385" s="6"/>
+      <c r="B385" s="7"/>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A386" s="6"/>
+      <c r="B386" s="7"/>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A387" s="6"/>
+      <c r="B387" s="7"/>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A388" s="6"/>
+      <c r="B388" s="7"/>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A389" s="6"/>
+      <c r="B389" s="7"/>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A390" s="6"/>
+      <c r="B390" s="7"/>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A391" s="6"/>
+      <c r="B391" s="7"/>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A392" s="6"/>
+      <c r="B392" s="7"/>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A393" s="6"/>
+      <c r="B393" s="7"/>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A394" s="6"/>
+      <c r="B394" s="7"/>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A395" s="6"/>
+      <c r="B395" s="7"/>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A396" s="6"/>
+      <c r="B396" s="7"/>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A397" s="6"/>
+      <c r="B397" s="7"/>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A398" s="6"/>
+      <c r="B398" s="7"/>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A399" s="6"/>
+      <c r="B399" s="7"/>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A400" s="6"/>
+      <c r="B400" s="7"/>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A401" s="6"/>
+      <c r="B401" s="7"/>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A402" s="6"/>
+      <c r="B402" s="7"/>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A403" s="6"/>
+      <c r="B403" s="7"/>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A404" s="6"/>
+      <c r="B404" s="7"/>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A405" s="6"/>
+      <c r="B405" s="7"/>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A406" s="6"/>
+      <c r="B406" s="7"/>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A407" s="6"/>
+      <c r="B407" s="7"/>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A408" s="6"/>
+      <c r="B408" s="7"/>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A409" s="6"/>
+      <c r="B409" s="7"/>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A410" s="6"/>
+      <c r="B410" s="7"/>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A411" s="6"/>
+      <c r="B411" s="7"/>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A412" s="6"/>
+      <c r="B412" s="7"/>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A413" s="6"/>
+      <c r="B413" s="7"/>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A414" s="6"/>
+      <c r="B414" s="7"/>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A415" s="6"/>
+      <c r="B415" s="7"/>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A416" s="6"/>
+      <c r="B416" s="7"/>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A417" s="6"/>
+      <c r="B417" s="7"/>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A418" s="6"/>
+      <c r="B418" s="7"/>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A419" s="6"/>
+      <c r="B419" s="7"/>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A420" s="6"/>
+      <c r="B420" s="7"/>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A421" s="6"/>
+      <c r="B421" s="7"/>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A422" s="6"/>
+      <c r="B422" s="7"/>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A423" s="6"/>
+      <c r="B423" s="7"/>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A424" s="6"/>
+      <c r="B424" s="7"/>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A425" s="6"/>
+      <c r="B425" s="7"/>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A426" s="6"/>
+      <c r="B426" s="7"/>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A427" s="6"/>
+      <c r="B427" s="7"/>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A428" s="6"/>
+      <c r="B428" s="7"/>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A429" s="6"/>
+      <c r="B429" s="7"/>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A430" s="6"/>
+      <c r="B430" s="7"/>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A431" s="6"/>
+      <c r="B431" s="7"/>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A432" s="6"/>
+      <c r="B432" s="7"/>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A433" s="6"/>
+      <c r="B433" s="7"/>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A434" s="6"/>
+      <c r="B434" s="7"/>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A435" s="6"/>
+      <c r="B435" s="7"/>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A436" s="6"/>
+      <c r="B436" s="7"/>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A437" s="6"/>
+      <c r="B437" s="7"/>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A438" s="6"/>
+      <c r="B438" s="7"/>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A439" s="6"/>
+      <c r="B439" s="7"/>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A440" s="6"/>
+      <c r="B440" s="7"/>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A441" s="6"/>
+      <c r="B441" s="7"/>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A442" s="6"/>
+      <c r="B442" s="7"/>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A443" s="6"/>
+      <c r="B443" s="7"/>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A444" s="6"/>
+      <c r="B444" s="7"/>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A445" s="6"/>
+      <c r="B445" s="7"/>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A446" s="6"/>
+      <c r="B446" s="7"/>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A447" s="6"/>
+      <c r="B447" s="7"/>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A448" s="6"/>
+      <c r="B448" s="7"/>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A449" s="6"/>
+      <c r="B449" s="7"/>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A450" s="6"/>
+      <c r="B450" s="7"/>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A451" s="6"/>
+      <c r="B451" s="7"/>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A452" s="6"/>
+      <c r="B452" s="7"/>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A453" s="6"/>
+      <c r="B453" s="7"/>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A454" s="6"/>
+      <c r="B454" s="7"/>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A455" s="6"/>
+      <c r="B455" s="7"/>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A456" s="6"/>
+      <c r="B456" s="7"/>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A457" s="6"/>
+      <c r="B457" s="7"/>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A458" s="6"/>
+      <c r="B458" s="7"/>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A459" s="6"/>
+      <c r="B459" s="7"/>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A460" s="6"/>
+      <c r="B460" s="7"/>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A461" s="6"/>
+      <c r="B461" s="7"/>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A462" s="6"/>
+      <c r="B462" s="7"/>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A463" s="6"/>
+      <c r="B463" s="7"/>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A464" s="6"/>
+      <c r="B464" s="7"/>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A465" s="6"/>
+      <c r="B465" s="7"/>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A466" s="6"/>
+      <c r="B466" s="7"/>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A467" s="6"/>
+      <c r="B467" s="7"/>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A468" s="6"/>
+      <c r="B468" s="7"/>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A469" s="6"/>
+      <c r="B469" s="7"/>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A470" s="6"/>
+      <c r="B470" s="7"/>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A471" s="6"/>
+      <c r="B471" s="7"/>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A472" s="6"/>
+      <c r="B472" s="7"/>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A473" s="6"/>
+      <c r="B473" s="7"/>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A474" s="6"/>
+      <c r="B474" s="7"/>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A475" s="6"/>
+      <c r="B475" s="7"/>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A476" s="6"/>
+      <c r="B476" s="7"/>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A477" s="6"/>
+      <c r="B477" s="7"/>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A478" s="6"/>
+      <c r="B478" s="7"/>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A479" s="6"/>
       <c r="B479" s="7"/>
     </row>
-    <row r="480" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A480" s="6"/>
       <c r="B480" s="7"/>
     </row>
@@ -4431,478 +3989,6 @@
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A773" s="6"/>
-      <c r="B773" s="7"/>
-    </row>
-    <row r="774" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A774" s="6"/>
-      <c r="B774" s="7"/>
-    </row>
-    <row r="775" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A775" s="6"/>
-      <c r="B775" s="7"/>
-    </row>
-    <row r="776" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A776" s="6"/>
-      <c r="B776" s="7"/>
-    </row>
-    <row r="777" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A777" s="6"/>
-      <c r="B777" s="7"/>
-    </row>
-    <row r="778" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A778" s="6"/>
-      <c r="B778" s="7"/>
-    </row>
-    <row r="779" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A779" s="6"/>
-      <c r="B779" s="7"/>
-    </row>
-    <row r="780" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A780" s="6"/>
-      <c r="B780" s="7"/>
-    </row>
-    <row r="781" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A781" s="6"/>
-      <c r="B781" s="7"/>
-    </row>
-    <row r="782" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A782" s="6"/>
-      <c r="B782" s="7"/>
-    </row>
-    <row r="783" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A783" s="6"/>
-      <c r="B783" s="7"/>
-    </row>
-    <row r="784" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A784" s="6"/>
-      <c r="B784" s="7"/>
-    </row>
-    <row r="785" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A785" s="6"/>
-      <c r="B785" s="7"/>
-    </row>
-    <row r="786" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A786" s="6"/>
-      <c r="B786" s="7"/>
-    </row>
-    <row r="787" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A787" s="6"/>
-      <c r="B787" s="7"/>
-    </row>
-    <row r="788" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A788" s="6"/>
-      <c r="B788" s="7"/>
-    </row>
-    <row r="789" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A789" s="6"/>
-      <c r="B789" s="7"/>
-    </row>
-    <row r="790" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A790" s="6"/>
-      <c r="B790" s="7"/>
-    </row>
-    <row r="791" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A791" s="6"/>
-      <c r="B791" s="7"/>
-    </row>
-    <row r="792" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A792" s="6"/>
-      <c r="B792" s="7"/>
-    </row>
-    <row r="793" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A793" s="6"/>
-      <c r="B793" s="7"/>
-    </row>
-    <row r="794" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A794" s="6"/>
-      <c r="B794" s="7"/>
-    </row>
-    <row r="795" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A795" s="6"/>
-      <c r="B795" s="7"/>
-    </row>
-    <row r="796" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A796" s="6"/>
-      <c r="B796" s="7"/>
-    </row>
-    <row r="797" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A797" s="6"/>
-      <c r="B797" s="7"/>
-    </row>
-    <row r="798" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A798" s="6"/>
-      <c r="B798" s="7"/>
-    </row>
-    <row r="799" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A799" s="6"/>
-      <c r="B799" s="7"/>
-    </row>
-    <row r="800" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A800" s="6"/>
-      <c r="B800" s="7"/>
-    </row>
-    <row r="801" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A801" s="6"/>
-      <c r="B801" s="7"/>
-    </row>
-    <row r="802" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A802" s="6"/>
-      <c r="B802" s="7"/>
-    </row>
-    <row r="803" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A803" s="6"/>
-      <c r="B803" s="7"/>
-    </row>
-    <row r="804" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A804" s="6"/>
-      <c r="B804" s="7"/>
-    </row>
-    <row r="805" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A805" s="6"/>
-      <c r="B805" s="7"/>
-    </row>
-    <row r="806" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A806" s="6"/>
-      <c r="B806" s="7"/>
-    </row>
-    <row r="807" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A807" s="6"/>
-      <c r="B807" s="7"/>
-    </row>
-    <row r="808" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A808" s="6"/>
-      <c r="B808" s="7"/>
-    </row>
-    <row r="809" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A809" s="6"/>
-      <c r="B809" s="7"/>
-    </row>
-    <row r="810" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A810" s="6"/>
-      <c r="B810" s="7"/>
-    </row>
-    <row r="811" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A811" s="6"/>
-      <c r="B811" s="7"/>
-    </row>
-    <row r="812" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A812" s="6"/>
-      <c r="B812" s="7"/>
-    </row>
-    <row r="813" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A813" s="6"/>
-      <c r="B813" s="7"/>
-    </row>
-    <row r="814" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A814" s="6"/>
-      <c r="B814" s="7"/>
-    </row>
-    <row r="815" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A815" s="6"/>
-      <c r="B815" s="7"/>
-    </row>
-    <row r="816" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A816" s="6"/>
-      <c r="B816" s="7"/>
-    </row>
-    <row r="817" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A817" s="6"/>
-      <c r="B817" s="7"/>
-    </row>
-    <row r="818" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A818" s="6"/>
-      <c r="B818" s="7"/>
-    </row>
-    <row r="819" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A819" s="6"/>
-      <c r="B819" s="7"/>
-    </row>
-    <row r="820" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A820" s="6"/>
-      <c r="B820" s="7"/>
-    </row>
-    <row r="821" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A821" s="6"/>
-      <c r="B821" s="7"/>
-    </row>
-    <row r="822" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A822" s="6"/>
-      <c r="B822" s="7"/>
-    </row>
-    <row r="823" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A823" s="6"/>
-      <c r="B823" s="7"/>
-    </row>
-    <row r="824" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A824" s="6"/>
-      <c r="B824" s="7"/>
-    </row>
-    <row r="825" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A825" s="6"/>
-      <c r="B825" s="7"/>
-    </row>
-    <row r="826" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A826" s="6"/>
-      <c r="B826" s="7"/>
-    </row>
-    <row r="827" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A827" s="6"/>
-      <c r="B827" s="7"/>
-    </row>
-    <row r="828" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A828" s="6"/>
-      <c r="B828" s="7"/>
-    </row>
-    <row r="829" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A829" s="6"/>
-      <c r="B829" s="7"/>
-    </row>
-    <row r="830" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A830" s="6"/>
-      <c r="B830" s="7"/>
-    </row>
-    <row r="831" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A831" s="6"/>
-      <c r="B831" s="7"/>
-    </row>
-    <row r="832" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A832" s="6"/>
-      <c r="B832" s="7"/>
-    </row>
-    <row r="833" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A833" s="6"/>
-      <c r="B833" s="7"/>
-    </row>
-    <row r="834" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A834" s="6"/>
-      <c r="B834" s="7"/>
-    </row>
-    <row r="835" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A835" s="6"/>
-      <c r="B835" s="7"/>
-    </row>
-    <row r="836" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A836" s="6"/>
-      <c r="B836" s="7"/>
-    </row>
-    <row r="837" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A837" s="6"/>
-      <c r="B837" s="7"/>
-    </row>
-    <row r="838" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A838" s="6"/>
-      <c r="B838" s="7"/>
-    </row>
-    <row r="839" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A839" s="6"/>
-      <c r="B839" s="7"/>
-    </row>
-    <row r="840" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A840" s="6"/>
-      <c r="B840" s="7"/>
-    </row>
-    <row r="841" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A841" s="6"/>
-      <c r="B841" s="7"/>
-    </row>
-    <row r="842" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A842" s="6"/>
-      <c r="B842" s="7"/>
-    </row>
-    <row r="843" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A843" s="6"/>
-      <c r="B843" s="7"/>
-    </row>
-    <row r="844" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A844" s="6"/>
-      <c r="B844" s="7"/>
-    </row>
-    <row r="845" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A845" s="6"/>
-      <c r="B845" s="7"/>
-    </row>
-    <row r="846" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A846" s="6"/>
-      <c r="B846" s="7"/>
-    </row>
-    <row r="847" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A847" s="6"/>
-      <c r="B847" s="7"/>
-    </row>
-    <row r="848" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A848" s="6"/>
-      <c r="B848" s="7"/>
-    </row>
-    <row r="849" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A849" s="6"/>
-      <c r="B849" s="7"/>
-    </row>
-    <row r="850" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A850" s="6"/>
-      <c r="B850" s="7"/>
-    </row>
-    <row r="851" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A851" s="6"/>
-      <c r="B851" s="7"/>
-    </row>
-    <row r="852" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A852" s="6"/>
-      <c r="B852" s="7"/>
-    </row>
-    <row r="853" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A853" s="6"/>
-      <c r="B853" s="7"/>
-    </row>
-    <row r="854" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A854" s="6"/>
-      <c r="B854" s="7"/>
-    </row>
-    <row r="855" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A855" s="6"/>
-      <c r="B855" s="7"/>
-    </row>
-    <row r="856" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A856" s="6"/>
-      <c r="B856" s="7"/>
-    </row>
-    <row r="857" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A857" s="6"/>
-      <c r="B857" s="7"/>
-    </row>
-    <row r="858" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A858" s="6"/>
-      <c r="B858" s="7"/>
-    </row>
-    <row r="859" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A859" s="6"/>
-      <c r="B859" s="7"/>
-    </row>
-    <row r="860" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A860" s="6"/>
-      <c r="B860" s="7"/>
-    </row>
-    <row r="861" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A861" s="6"/>
-      <c r="B861" s="7"/>
-    </row>
-    <row r="862" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A862" s="6"/>
-      <c r="B862" s="7"/>
-    </row>
-    <row r="863" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A863" s="6"/>
-      <c r="B863" s="7"/>
-    </row>
-    <row r="864" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A864" s="6"/>
-      <c r="B864" s="7"/>
-    </row>
-    <row r="865" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A865" s="6"/>
-      <c r="B865" s="7"/>
-    </row>
-    <row r="866" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A866" s="6"/>
-      <c r="B866" s="7"/>
-    </row>
-    <row r="867" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A867" s="6"/>
-      <c r="B867" s="7"/>
-    </row>
-    <row r="868" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A868" s="6"/>
-      <c r="B868" s="7"/>
-    </row>
-    <row r="869" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A869" s="6"/>
-      <c r="B869" s="7"/>
-    </row>
-    <row r="870" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A870" s="6"/>
-      <c r="B870" s="7"/>
-    </row>
-    <row r="871" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A871" s="6"/>
-      <c r="B871" s="7"/>
-    </row>
-    <row r="872" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A872" s="6"/>
-      <c r="B872" s="7"/>
-    </row>
-    <row r="873" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A873" s="6"/>
-      <c r="B873" s="7"/>
-    </row>
-    <row r="874" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A874" s="6"/>
-      <c r="B874" s="7"/>
-    </row>
-    <row r="875" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A875" s="6"/>
-      <c r="B875" s="7"/>
-    </row>
-    <row r="876" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A876" s="6"/>
-      <c r="B876" s="7"/>
-    </row>
-    <row r="877" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A877" s="6"/>
-      <c r="B877" s="7"/>
-    </row>
-    <row r="878" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A878" s="6"/>
-      <c r="B878" s="7"/>
-    </row>
-    <row r="879" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A879" s="6"/>
-      <c r="B879" s="7"/>
-    </row>
-    <row r="880" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A880" s="6"/>
-      <c r="B880" s="7"/>
-    </row>
-    <row r="881" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A881" s="6"/>
-      <c r="B881" s="7"/>
-    </row>
-    <row r="882" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A882" s="6"/>
-      <c r="B882" s="7"/>
-    </row>
-    <row r="883" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A883" s="6"/>
-      <c r="B883" s="7"/>
-    </row>
-    <row r="884" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A884" s="6"/>
-      <c r="B884" s="7"/>
-    </row>
-    <row r="885" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A885" s="6"/>
-      <c r="B885" s="7"/>
-    </row>
-    <row r="886" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A886" s="6"/>
-      <c r="B886" s="7"/>
-    </row>
-    <row r="887" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A887" s="6"/>
-      <c r="B887" s="7"/>
-    </row>
-    <row r="888" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A888" s="6"/>
-      <c r="B888" s="7"/>
-    </row>
-    <row r="889" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A889" s="6"/>
-      <c r="B889" s="7"/>
-    </row>
-    <row r="890" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A890" s="6"/>
-      <c r="B890" s="7"/>
-    </row>
-    <row r="891" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A891" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
correção na leitura do config
</commit_message>
<xml_diff>
--- a/bot/Assets/IO/Input/Execucao.xlsx
+++ b/bot/Assets/IO/Input/Execucao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bot-clicker-orcamento\bot\Assets\IO\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Produto</t>
   </si>
@@ -32,16 +32,7 @@
     <t>Quantidade</t>
   </si>
   <si>
-    <t>LACTOBACILUS CASEI</t>
-  </si>
-  <si>
-    <t>LACTOBACILUS PLANTARUM</t>
-  </si>
-  <si>
-    <t>LACTOBACILUS SALIVARIUM</t>
-  </si>
-  <si>
-    <t>PIRIDOXINA</t>
+    <t>gelatina</t>
   </si>
 </sst>
 </file>
@@ -511,7 +502,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I773"/>
+  <dimension ref="A1:I772"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -536,36 +527,28 @@
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="15"/>
       <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="10"/>
       <c r="B3" s="15"/>
       <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="10"/>
       <c r="B4" s="15"/>
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="10"/>
       <c r="B5" s="15"/>
       <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="10"/>
       <c r="B6" s="15"/>
       <c r="I6" s="18"/>
     </row>
@@ -1875,22 +1858,22 @@
       <c r="I267" s="18"/>
     </row>
     <row r="268" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="10"/>
+      <c r="A268" s="11"/>
       <c r="B268" s="15"/>
       <c r="I268" s="18"/>
     </row>
     <row r="269" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A269" s="10"/>
+      <c r="A269" s="2"/>
       <c r="B269" s="15"/>
       <c r="I269" s="18"/>
     </row>
     <row r="270" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A270" s="10"/>
+      <c r="A270" s="2"/>
       <c r="B270" s="2"/>
       <c r="I270" s="18"/>
     </row>
     <row r="271" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="11"/>
+      <c r="A271" s="2"/>
       <c r="B271" s="2"/>
       <c r="I271" s="18"/>
     </row>
@@ -2205,7 +2188,7 @@
       <c r="I333" s="18"/>
     </row>
     <row r="334" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A334" s="2"/>
+      <c r="A334" s="12"/>
       <c r="B334" s="16"/>
       <c r="I334" s="18"/>
     </row>
@@ -2220,12 +2203,12 @@
       <c r="I336" s="18"/>
     </row>
     <row r="337" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A337" s="12"/>
+      <c r="A337" s="11"/>
       <c r="B337" s="2"/>
       <c r="I337" s="18"/>
     </row>
     <row r="338" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A338" s="2"/>
+      <c r="A338" s="13"/>
       <c r="B338" s="16"/>
       <c r="I338" s="18"/>
     </row>
@@ -2235,12 +2218,12 @@
       <c r="I339" s="18"/>
     </row>
     <row r="340" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A340" s="11"/>
+      <c r="A340" s="2"/>
       <c r="B340" s="2"/>
       <c r="I340" s="18"/>
     </row>
     <row r="341" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A341" s="13"/>
+      <c r="A341" s="2"/>
       <c r="B341" s="2"/>
       <c r="I341" s="18"/>
     </row>
@@ -2250,7 +2233,7 @@
       <c r="I342" s="18"/>
     </row>
     <row r="343" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A343" s="2"/>
+      <c r="A343" s="10"/>
       <c r="B343" s="16"/>
       <c r="I343" s="18"/>
     </row>
@@ -2265,7 +2248,7 @@
       <c r="I345" s="18"/>
     </row>
     <row r="346" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A346" s="10"/>
+      <c r="A346" s="2"/>
       <c r="B346" s="16"/>
       <c r="I346" s="18"/>
     </row>
@@ -2300,7 +2283,7 @@
       <c r="I352" s="18"/>
     </row>
     <row r="353" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A353" s="2"/>
+      <c r="A353" s="10"/>
       <c r="B353" s="12"/>
       <c r="I353" s="18"/>
     </row>
@@ -2310,12 +2293,12 @@
       <c r="I354" s="18"/>
     </row>
     <row r="355" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A355" s="2"/>
+      <c r="A355" s="13"/>
       <c r="B355" s="2"/>
       <c r="I355" s="18"/>
     </row>
     <row r="356" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A356" s="10"/>
+      <c r="A356" s="14"/>
       <c r="B356" s="16"/>
       <c r="I356" s="18"/>
     </row>
@@ -2325,22 +2308,22 @@
       <c r="I357" s="18"/>
     </row>
     <row r="358" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A358" s="13"/>
+      <c r="A358" s="10"/>
       <c r="B358" s="12"/>
       <c r="I358" s="18"/>
     </row>
     <row r="359" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A359" s="14"/>
+      <c r="A359" s="6"/>
       <c r="B359" s="16"/>
       <c r="I359" s="18"/>
     </row>
     <row r="360" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A360" s="2"/>
+      <c r="A360" s="6"/>
       <c r="B360" s="2"/>
       <c r="I360" s="18"/>
     </row>
-    <row r="361" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A361" s="10"/>
+    <row r="361" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A361" s="6"/>
       <c r="B361" s="7"/>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.3">
@@ -3980,15 +3963,10 @@
       <c r="B770" s="7"/>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A771" s="6"/>
       <c r="B771" s="7"/>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A772" s="6"/>
       <c r="B772" s="7"/>
-    </row>
-    <row r="773" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A773" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>